<commit_message>
Integrate Agora data for hydgn/BHPSbP, io-model/WMITR, and land/BLAPE
</commit_message>
<xml_diff>
--- a/InputData/hydgn/BHPSbP/BAU Hydrogen Production Shr by Pathway.xlsx
+++ b/InputData/hydgn/BHPSbP/BAU Hydrogen Production Shr by Pathway.xlsx
@@ -1,24 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\hydgn\BHPSbP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\hydgn\BHPSbP\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AB8A5A-B4F7-4257-97FF-6AED8EE9DB75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25815" windowHeight="11970"/>
+    <workbookView xWindow="40170" yWindow="5130" windowWidth="20625" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BHPSbP" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -48,18 +58,6 @@
     <t>biomass gasification</t>
   </si>
   <si>
-    <t>U.S. Department of Energy Fuel Cell Technologies Office</t>
-  </si>
-  <si>
-    <t>Hydrogen Production Processes</t>
-  </si>
-  <si>
-    <t>https://www.energy.gov/eere/fuelcells/hydrogen-production-processes</t>
-  </si>
-  <si>
-    <t>See sub-pages for each process, particularly "natural gas reforming"</t>
-  </si>
-  <si>
     <t>For international (global) statistics, see:</t>
   </si>
   <si>
@@ -85,12 +83,24 @@
   </si>
   <si>
     <t>Production Share (dimensionless)</t>
+  </si>
+  <si>
+    <t>European Commission</t>
+  </si>
+  <si>
+    <t>https://op.europa.eu/en/publication-detail/-/publication/7e4afa7d-d077-11ea-adf7-01aa75ed71a1</t>
+  </si>
+  <si>
+    <t>Hydrogen generation in Europe: Overview of costs and key benefits</t>
+  </si>
+  <si>
+    <t>Introduction (paragraphs 3 and 4)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,14 +437,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.73046875" customWidth="1"/>
+    <col min="1" max="1" width="12.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
@@ -447,27 +459,27 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="3">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
@@ -477,32 +489,32 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B19" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
@@ -527,13 +539,13 @@
         <v>0.22</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B19" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -541,22 +553,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="30.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2">
         <v>2017</v>
@@ -1223,7 +1237,7 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>0</v>

</xml_diff>

<commit_message>
Fix BHPSbP - byproduct H2 should not be accounted for within this file, as secondary fuels in industry aren't demanded in H2 sector
</commit_message>
<xml_diff>
--- a/InputData/hydgn/BHPSbP/BAU Hydrogen Production Shr by Pathway.xlsx
+++ b/InputData/hydgn/BHPSbP/BAU Hydrogen Production Shr by Pathway.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://artelys778.sharepoint.com/sites/Agora-EPStool-Artelys/Documents partages/Artelys/3 - Livrables/1. all data/2. A checker par Paul/13. BAU Hydrogen Production Shares by Pathway/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\hydgn\BHPSbP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{50744115-75AC-4525-8E2A-8202EB70A612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2807D661-327B-4E8F-8E14-AAA950F03467}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE88A35-2775-4540-8644-26B5F73E5862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12855" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="5" xr2:uid="{507E633D-E752-41BB-B866-72E946289DF3}"/>
+    <workbookView xWindow="35595" yWindow="2730" windowWidth="21600" windowHeight="11175" activeTab="5" xr2:uid="{507E633D-E752-41BB-B866-72E946289DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="163">
   <si>
     <t>BHPSbP BAU Hydrogen Production Shares by Pathway</t>
   </si>
@@ -749,6 +749,9 @@
   <si>
     <t>natural gas reforming with CCS</t>
   </si>
+  <si>
+    <t>EI Note: byproduct H2 is accounted for in the industry sector, not demanded by H2 producers, so it is excluded from production pathways here in the final BHPSbP tab</t>
+  </si>
 </sst>
 </file>
 
@@ -765,7 +768,7 @@
     <numFmt numFmtId="171" formatCode="0.0%"/>
     <numFmt numFmtId="172" formatCode="0.000"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -958,6 +961,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1195,7 +1207,7 @@
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1383,6 +1395,12 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="21" fillId="8" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="21" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1395,18 +1413,13 @@
     <xf numFmtId="0" fontId="21" fillId="8" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="8" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -4289,9 +4302,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4329,7 +4342,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4435,7 +4448,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4577,7 +4590,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4591,24 +4604,24 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="10.85546875" style="3"/>
     <col min="3" max="3" width="62.140625" style="3" customWidth="1"/>
     <col min="4" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>1</v>
       </c>
@@ -4619,7 +4632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="4" t="s">
         <v>4</v>
@@ -4628,7 +4641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="4" t="s">
         <v>6</v>
@@ -4637,37 +4650,37 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="95" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="C17" s="96" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="95" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="95" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C20" s="95" t="s">
         <v>13</v>
       </c>
@@ -4688,13 +4701,13 @@
   <dimension ref="A1:AA135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="D86" sqref="D86"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="10.15"/>
+  <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72" style="18" customWidth="1"/>
     <col min="2" max="9" width="7.7109375" style="18" bestFit="1" customWidth="1"/>
@@ -4705,7 +4718,7 @@
     <col min="16" max="16384" width="9.7109375" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="26.25" customHeight="1">
+    <row r="1" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -4728,7 +4741,7 @@
       <c r="R1" s="17"/>
       <c r="S1" s="17"/>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="36"/>
       <c r="B2" s="37">
         <v>2005</v>
@@ -4775,7 +4788,7 @@
       <c r="R2" s="17"/>
       <c r="S2" s="17"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>18</v>
       </c>
@@ -4798,7 +4811,7 @@
       <c r="R3" s="17"/>
       <c r="S3" s="17"/>
     </row>
-    <row r="4" spans="1:19" ht="11.25" customHeight="1">
+    <row r="4" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
         <v>19</v>
       </c>
@@ -4847,7 +4860,7 @@
       <c r="R4" s="17"/>
       <c r="S4" s="17"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
         <v>20</v>
       </c>
@@ -4896,7 +4909,7 @@
       <c r="R5" s="17"/>
       <c r="S5" s="17"/>
     </row>
-    <row r="6" spans="1:19" ht="12.75" customHeight="1">
+    <row r="6" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>21</v>
       </c>
@@ -4945,7 +4958,7 @@
       <c r="R6" s="17"/>
       <c r="S6" s="17"/>
     </row>
-    <row r="7" spans="1:19" ht="12.75" customHeight="1">
+    <row r="7" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
         <v>22</v>
       </c>
@@ -4994,7 +5007,7 @@
       <c r="R7" s="17"/>
       <c r="S7" s="17"/>
     </row>
-    <row r="8" spans="1:19" ht="12.75" customHeight="1">
+    <row r="8" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
         <v>23</v>
       </c>
@@ -5043,7 +5056,7 @@
       <c r="R8" s="17"/>
       <c r="S8" s="17"/>
     </row>
-    <row r="9" spans="1:19" ht="11.25" customHeight="1">
+    <row r="9" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="43"/>
       <c r="B9" s="42"/>
       <c r="C9" s="42"/>
@@ -5064,7 +5077,7 @@
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
     </row>
-    <row r="10" spans="1:19" ht="12.75" customHeight="1">
+    <row r="10" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
         <v>24</v>
       </c>
@@ -5087,7 +5100,7 @@
       <c r="R10" s="17"/>
       <c r="S10" s="17"/>
     </row>
-    <row r="11" spans="1:19" ht="11.45">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
         <v>25</v>
       </c>
@@ -5136,7 +5149,7 @@
       <c r="R11" s="17"/>
       <c r="S11" s="17"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>26</v>
       </c>
@@ -5185,7 +5198,7 @@
       <c r="R12" s="17"/>
       <c r="S12" s="17"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="49" t="s">
         <v>27</v>
       </c>
@@ -5234,7 +5247,7 @@
       <c r="R13" s="17"/>
       <c r="S13" s="17"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="49" t="s">
         <v>28</v>
       </c>
@@ -5283,7 +5296,7 @@
       <c r="R14" s="17"/>
       <c r="S14" s="17"/>
     </row>
-    <row r="15" spans="1:19" ht="11.45">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
         <v>29</v>
       </c>
@@ -5328,7 +5341,7 @@
       <c r="R15" s="17"/>
       <c r="S15" s="17"/>
     </row>
-    <row r="16" spans="1:19" ht="11.45">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
         <v>31</v>
       </c>
@@ -5377,7 +5390,7 @@
       <c r="R16" s="17"/>
       <c r="S16" s="17"/>
     </row>
-    <row r="17" spans="1:19" ht="11.45">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
         <v>32</v>
       </c>
@@ -5426,7 +5439,7 @@
       <c r="R17" s="17"/>
       <c r="S17" s="17"/>
     </row>
-    <row r="18" spans="1:19" ht="11.45">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="47" t="s">
         <v>33</v>
       </c>
@@ -5475,7 +5488,7 @@
       <c r="R18" s="17"/>
       <c r="S18" s="17"/>
     </row>
-    <row r="19" spans="1:19" ht="12.75" customHeight="1">
+    <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
         <v>35</v>
       </c>
@@ -5524,7 +5537,7 @@
       <c r="R19" s="17"/>
       <c r="S19" s="17"/>
     </row>
-    <row r="20" spans="1:19" ht="12" customHeight="1">
+    <row r="20" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="43"/>
       <c r="B20" s="42"/>
       <c r="C20" s="42"/>
@@ -5545,7 +5558,7 @@
       <c r="R20" s="17"/>
       <c r="S20" s="17"/>
     </row>
-    <row r="21" spans="1:19" ht="12.75" customHeight="1">
+    <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
         <v>36</v>
       </c>
@@ -5568,7 +5581,7 @@
       <c r="R21" s="17"/>
       <c r="S21" s="17"/>
     </row>
-    <row r="22" spans="1:19" ht="12.75" customHeight="1">
+    <row r="22" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="54" t="s">
         <v>37</v>
       </c>
@@ -5617,7 +5630,7 @@
       <c r="R22" s="17"/>
       <c r="S22" s="17"/>
     </row>
-    <row r="23" spans="1:19" ht="12.75" customHeight="1">
+    <row r="23" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="49" t="s">
         <v>38</v>
       </c>
@@ -5666,7 +5679,7 @@
       <c r="R23" s="17"/>
       <c r="S23" s="17"/>
     </row>
-    <row r="24" spans="1:19" ht="12.75" customHeight="1">
+    <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="49" t="s">
         <v>39</v>
       </c>
@@ -5715,7 +5728,7 @@
       <c r="R24" s="17"/>
       <c r="S24" s="17"/>
     </row>
-    <row r="25" spans="1:19" ht="12.75" customHeight="1">
+    <row r="25" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="49" t="s">
         <v>40</v>
       </c>
@@ -5764,7 +5777,7 @@
       <c r="R25" s="17"/>
       <c r="S25" s="17"/>
     </row>
-    <row r="26" spans="1:19" ht="12.75" customHeight="1">
+    <row r="26" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="49" t="s">
         <v>41</v>
       </c>
@@ -5813,7 +5826,7 @@
       <c r="R26" s="17"/>
       <c r="S26" s="17"/>
     </row>
-    <row r="27" spans="1:19" ht="12.75" customHeight="1">
+    <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="51" t="s">
         <v>42</v>
       </c>
@@ -5862,7 +5875,7 @@
       <c r="R27" s="17"/>
       <c r="S27" s="17"/>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="49" t="s">
         <v>43</v>
       </c>
@@ -5911,7 +5924,7 @@
       <c r="R28" s="17"/>
       <c r="S28" s="17"/>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="49" t="s">
         <v>44</v>
       </c>
@@ -5960,7 +5973,7 @@
       <c r="R29" s="17"/>
       <c r="S29" s="17"/>
     </row>
-    <row r="30" spans="1:19" ht="12.75" customHeight="1">
+    <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="49" t="s">
         <v>45</v>
       </c>
@@ -6009,7 +6022,7 @@
       <c r="R30" s="17"/>
       <c r="S30" s="17"/>
     </row>
-    <row r="31" spans="1:19" ht="12.75" customHeight="1">
+    <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="49" t="s">
         <v>46</v>
       </c>
@@ -6058,7 +6071,7 @@
       <c r="R31" s="17"/>
       <c r="S31" s="17"/>
     </row>
-    <row r="32" spans="1:19" ht="12.75" customHeight="1">
+    <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="49" t="s">
         <v>47</v>
       </c>
@@ -6107,7 +6120,7 @@
       <c r="R32" s="17"/>
       <c r="S32" s="17"/>
     </row>
-    <row r="33" spans="1:19" ht="12.75" customHeight="1">
+    <row r="33" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="49" t="s">
         <v>48</v>
       </c>
@@ -6156,7 +6169,7 @@
       <c r="R33" s="17"/>
       <c r="S33" s="17"/>
     </row>
-    <row r="34" spans="1:19" ht="12" customHeight="1">
+    <row r="34" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="59"/>
       <c r="B34" s="42"/>
       <c r="C34" s="42"/>
@@ -6177,7 +6190,7 @@
       <c r="R34" s="17"/>
       <c r="S34" s="17"/>
     </row>
-    <row r="35" spans="1:19" ht="12.75" customHeight="1">
+    <row r="35" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="s">
         <v>49</v>
       </c>
@@ -6226,7 +6239,7 @@
       <c r="R35" s="17"/>
       <c r="S35" s="17"/>
     </row>
-    <row r="36" spans="1:19" ht="12.75" customHeight="1">
+    <row r="36" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="60" t="s">
         <v>50</v>
       </c>
@@ -6249,7 +6262,7 @@
       <c r="R36" s="17"/>
       <c r="S36" s="17"/>
     </row>
-    <row r="37" spans="1:19" ht="12.75" customHeight="1">
+    <row r="37" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="49" t="s">
         <v>51</v>
       </c>
@@ -6298,7 +6311,7 @@
       <c r="R37" s="17"/>
       <c r="S37" s="17"/>
     </row>
-    <row r="38" spans="1:19" ht="12.75" customHeight="1">
+    <row r="38" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="61" t="s">
         <v>52</v>
       </c>
@@ -6347,7 +6360,7 @@
       <c r="R38" s="17"/>
       <c r="S38" s="17"/>
     </row>
-    <row r="39" spans="1:19" ht="12.75" customHeight="1">
+    <row r="39" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="62" t="s">
         <v>53</v>
       </c>
@@ -6396,7 +6409,7 @@
       <c r="R39" s="17"/>
       <c r="S39" s="17"/>
     </row>
-    <row r="40" spans="1:19" ht="12.75" customHeight="1">
+    <row r="40" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="49" t="s">
         <v>54</v>
       </c>
@@ -6445,7 +6458,7 @@
       <c r="R40" s="17"/>
       <c r="S40" s="17"/>
     </row>
-    <row r="41" spans="1:19" ht="12.75" customHeight="1">
+    <row r="41" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="51" t="s">
         <v>55</v>
       </c>
@@ -6494,7 +6507,7 @@
       <c r="R41" s="17"/>
       <c r="S41" s="17"/>
     </row>
-    <row r="42" spans="1:19" ht="12.75" customHeight="1">
+    <row r="42" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="51" t="s">
         <v>56</v>
       </c>
@@ -6543,7 +6556,7 @@
       <c r="R42" s="17"/>
       <c r="S42" s="17"/>
     </row>
-    <row r="43" spans="1:19" ht="12.75" customHeight="1">
+    <row r="43" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="60" t="s">
         <v>57</v>
       </c>
@@ -6566,7 +6579,7 @@
       <c r="R43" s="17"/>
       <c r="S43" s="17"/>
     </row>
-    <row r="44" spans="1:19" ht="12.75" customHeight="1">
+    <row r="44" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="49" t="s">
         <v>38</v>
       </c>
@@ -6615,7 +6628,7 @@
       <c r="R44" s="17"/>
       <c r="S44" s="17"/>
     </row>
-    <row r="45" spans="1:19" ht="12.75" customHeight="1">
+    <row r="45" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="49" t="s">
         <v>58</v>
       </c>
@@ -6664,7 +6677,7 @@
       <c r="R45" s="17"/>
       <c r="S45" s="17"/>
     </row>
-    <row r="46" spans="1:19" ht="12.75" customHeight="1">
+    <row r="46" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="49" t="s">
         <v>40</v>
       </c>
@@ -6713,7 +6726,7 @@
       <c r="R46" s="17"/>
       <c r="S46" s="17"/>
     </row>
-    <row r="47" spans="1:19" ht="12.75" customHeight="1">
+    <row r="47" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="49" t="s">
         <v>59</v>
       </c>
@@ -6762,7 +6775,7 @@
       <c r="R47" s="17"/>
       <c r="S47" s="17"/>
     </row>
-    <row r="48" spans="1:19" ht="12.75" customHeight="1">
+    <row r="48" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="49" t="s">
         <v>60</v>
       </c>
@@ -6811,7 +6824,7 @@
       <c r="R48" s="17"/>
       <c r="S48" s="17"/>
     </row>
-    <row r="49" spans="1:22" ht="12.75" customHeight="1">
+    <row r="49" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="49" t="s">
         <v>61</v>
       </c>
@@ -6860,7 +6873,7 @@
       <c r="R49" s="17"/>
       <c r="S49" s="17"/>
     </row>
-    <row r="50" spans="1:22" ht="11.45">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="61" t="s">
         <v>62</v>
       </c>
@@ -6909,7 +6922,7 @@
       <c r="R50" s="17"/>
       <c r="S50" s="17"/>
     </row>
-    <row r="51" spans="1:22">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="62" t="s">
         <v>63</v>
       </c>
@@ -6958,7 +6971,7 @@
       <c r="R51" s="17"/>
       <c r="S51" s="17"/>
     </row>
-    <row r="52" spans="1:22" ht="12.75" customHeight="1">
+    <row r="52" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="62" t="s">
         <v>64</v>
       </c>
@@ -7007,7 +7020,7 @@
       <c r="R52" s="17"/>
       <c r="S52" s="17"/>
     </row>
-    <row r="53" spans="1:22" ht="12.75" customHeight="1">
+    <row r="53" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="49" t="s">
         <v>65</v>
       </c>
@@ -7056,7 +7069,7 @@
       <c r="R53" s="17"/>
       <c r="S53" s="17"/>
     </row>
-    <row r="54" spans="1:22" ht="12.75" customHeight="1">
+    <row r="54" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="49" t="s">
         <v>66</v>
       </c>
@@ -7105,7 +7118,7 @@
       <c r="R54" s="17"/>
       <c r="S54" s="17"/>
     </row>
-    <row r="55" spans="1:22" ht="12" customHeight="1">
+    <row r="55" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="49"/>
       <c r="B55" s="56"/>
       <c r="C55" s="56"/>
@@ -7126,7 +7139,7 @@
       <c r="R55" s="17"/>
       <c r="S55" s="17"/>
     </row>
-    <row r="56" spans="1:22" ht="12.75" customHeight="1">
+    <row r="56" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="40" t="s">
         <v>67</v>
       </c>
@@ -7175,7 +7188,7 @@
       <c r="R56" s="17"/>
       <c r="S56" s="17"/>
     </row>
-    <row r="57" spans="1:22" ht="12" customHeight="1">
+    <row r="57" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="63"/>
       <c r="B57" s="64"/>
       <c r="C57" s="64"/>
@@ -7199,7 +7212,7 @@
       <c r="U57" s="25"/>
       <c r="V57" s="25"/>
     </row>
-    <row r="58" spans="1:22" ht="12.75" customHeight="1">
+    <row r="58" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="40" t="s">
         <v>68</v>
       </c>
@@ -7251,7 +7264,7 @@
       <c r="U58" s="25"/>
       <c r="V58" s="25"/>
     </row>
-    <row r="59" spans="1:22" ht="12.75" customHeight="1">
+    <row r="59" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="66" t="s">
         <v>69</v>
       </c>
@@ -7300,7 +7313,7 @@
       <c r="R59" s="25"/>
       <c r="S59" s="25"/>
     </row>
-    <row r="60" spans="1:22" ht="12.75" customHeight="1">
+    <row r="60" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="49" t="s">
         <v>38</v>
       </c>
@@ -7352,7 +7365,7 @@
       <c r="U60" s="27"/>
       <c r="V60" s="27"/>
     </row>
-    <row r="61" spans="1:22" ht="12.75" customHeight="1">
+    <row r="61" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="49" t="s">
         <v>58</v>
       </c>
@@ -7404,7 +7417,7 @@
       <c r="U61" s="27"/>
       <c r="V61" s="27"/>
     </row>
-    <row r="62" spans="1:22" ht="12.75" customHeight="1">
+    <row r="62" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="49" t="s">
         <v>40</v>
       </c>
@@ -7453,7 +7466,7 @@
       <c r="R62" s="27"/>
       <c r="S62" s="27"/>
     </row>
-    <row r="63" spans="1:22" ht="12.75" customHeight="1">
+    <row r="63" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="49" t="s">
         <v>41</v>
       </c>
@@ -7502,7 +7515,7 @@
       <c r="R63" s="25"/>
       <c r="S63" s="25"/>
     </row>
-    <row r="64" spans="1:22" ht="12.75" customHeight="1">
+    <row r="64" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="49" t="s">
         <v>70</v>
       </c>
@@ -7551,7 +7564,7 @@
       <c r="R64" s="25"/>
       <c r="S64" s="25"/>
     </row>
-    <row r="65" spans="1:27" ht="12.75" customHeight="1">
+    <row r="65" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="51" t="s">
         <v>42</v>
       </c>
@@ -7600,7 +7613,7 @@
       <c r="R65" s="27"/>
       <c r="S65" s="27"/>
     </row>
-    <row r="66" spans="1:27" ht="12.75" customHeight="1">
+    <row r="66" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="49" t="s">
         <v>71</v>
       </c>
@@ -7649,7 +7662,7 @@
       <c r="R66" s="17"/>
       <c r="S66" s="17"/>
     </row>
-    <row r="67" spans="1:27" ht="12.75" customHeight="1">
+    <row r="67" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="49" t="s">
         <v>65</v>
       </c>
@@ -7698,7 +7711,7 @@
       <c r="R67" s="25"/>
       <c r="S67" s="25"/>
     </row>
-    <row r="68" spans="1:27" ht="12.75" customHeight="1">
+    <row r="68" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="49" t="s">
         <v>66</v>
       </c>
@@ -7747,7 +7760,7 @@
       <c r="R68" s="25"/>
       <c r="S68" s="25"/>
     </row>
-    <row r="69" spans="1:27" ht="12.75" customHeight="1">
+    <row r="69" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="49" t="s">
         <v>59</v>
       </c>
@@ -7796,7 +7809,7 @@
       <c r="R69" s="25"/>
       <c r="S69" s="25"/>
     </row>
-    <row r="70" spans="1:27">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" s="66" t="s">
         <v>72</v>
       </c>
@@ -7845,7 +7858,7 @@
       <c r="R70" s="17"/>
       <c r="S70" s="17"/>
     </row>
-    <row r="71" spans="1:27" ht="12.75" customHeight="1">
+    <row r="71" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="66" t="s">
         <v>73</v>
       </c>
@@ -7894,7 +7907,7 @@
       <c r="R71" s="17"/>
       <c r="S71" s="17"/>
     </row>
-    <row r="72" spans="1:27">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" s="49" t="s">
         <v>65</v>
       </c>
@@ -7943,7 +7956,7 @@
       <c r="R72" s="17"/>
       <c r="S72" s="17"/>
     </row>
-    <row r="73" spans="1:27">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" s="49" t="s">
         <v>59</v>
       </c>
@@ -7992,7 +8005,7 @@
       <c r="R73" s="17"/>
       <c r="S73" s="17"/>
     </row>
-    <row r="74" spans="1:27" ht="12" customHeight="1" thickBot="1">
+    <row r="74" spans="1:27" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="63"/>
       <c r="B74" s="63"/>
       <c r="C74" s="63"/>
@@ -8031,7 +8044,7 @@
       <c r="Z74" s="81"/>
       <c r="AA74" s="81"/>
     </row>
-    <row r="75" spans="1:27" ht="12" customHeight="1" thickBot="1">
+    <row r="75" spans="1:27" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="79" t="s">
         <v>76</v>
       </c>
@@ -8086,7 +8099,7 @@
       <c r="R75" s="17"/>
       <c r="S75" s="17"/>
     </row>
-    <row r="76" spans="1:27">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" s="40" t="s">
         <v>78</v>
       </c>
@@ -8135,7 +8148,7 @@
       <c r="R76" s="17"/>
       <c r="S76" s="17"/>
     </row>
-    <row r="77" spans="1:27">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" s="66" t="s">
         <v>79</v>
       </c>
@@ -8184,7 +8197,7 @@
       <c r="R77" s="17"/>
       <c r="S77" s="17"/>
     </row>
-    <row r="78" spans="1:27">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" s="49" t="s">
         <v>59</v>
       </c>
@@ -8228,7 +8241,7 @@
         <v>0.78568541307690865</v>
       </c>
     </row>
-    <row r="79" spans="1:27">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" s="49" t="s">
         <v>80</v>
       </c>
@@ -8272,7 +8285,7 @@
         <v>-0.22262296039353702</v>
       </c>
     </row>
-    <row r="80" spans="1:27">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" s="66" t="s">
         <v>81</v>
       </c>
@@ -8316,7 +8329,7 @@
         <v>7.0438645968828872E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:19">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="66" t="s">
         <v>82</v>
       </c>
@@ -8360,7 +8373,7 @@
         <v>19.360960664325887</v>
       </c>
     </row>
-    <row r="82" spans="1:19">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="49" t="s">
         <v>83</v>
       </c>
@@ -8414,7 +8427,7 @@
       <c r="R82" s="93"/>
       <c r="S82" s="93"/>
     </row>
-    <row r="83" spans="1:19">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="49" t="s">
         <v>66</v>
       </c>
@@ -8458,7 +8471,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="12" customHeight="1">
+    <row r="84" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="49"/>
       <c r="B84" s="56"/>
       <c r="C84" s="56"/>
@@ -8474,7 +8487,7 @@
       <c r="M84" s="23"/>
       <c r="N84" s="23"/>
     </row>
-    <row r="85" spans="1:19">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="40" t="s">
         <v>85</v>
       </c>
@@ -8518,7 +8531,7 @@
         <v>-1.5118135951797562</v>
       </c>
     </row>
-    <row r="86" spans="1:19">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="49" t="s">
         <v>38</v>
       </c>
@@ -8562,7 +8575,7 @@
         <v>-4.3467157152702995</v>
       </c>
     </row>
-    <row r="87" spans="1:19">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="49" t="s">
         <v>39</v>
       </c>
@@ -8606,7 +8619,7 @@
         <v>-2.5140555801019593</v>
       </c>
     </row>
-    <row r="88" spans="1:19">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="49" t="s">
         <v>40</v>
       </c>
@@ -8650,7 +8663,7 @@
         <v>-0.5307788461428764</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="11.45">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="51" t="s">
         <v>86</v>
       </c>
@@ -8694,7 +8707,7 @@
         <v>-0.96420094272123835</v>
       </c>
     </row>
-    <row r="90" spans="1:19">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="49" t="s">
         <v>65</v>
       </c>
@@ -8738,7 +8751,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:19">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="49" t="s">
         <v>66</v>
       </c>
@@ -8782,7 +8795,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="1:19">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" s="49" t="s">
         <v>59</v>
       </c>
@@ -8826,7 +8839,7 @@
         <v>-1.6348708093032016</v>
       </c>
     </row>
-    <row r="93" spans="1:19">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" s="49" t="s">
         <v>80</v>
       </c>
@@ -8870,7 +8883,7 @@
         <v>-0.1333028156052074</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="12" customHeight="1">
+    <row r="94" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="49"/>
       <c r="B94" s="56"/>
       <c r="C94" s="56"/>
@@ -8886,7 +8899,7 @@
       <c r="M94" s="23"/>
       <c r="N94" s="23"/>
     </row>
-    <row r="95" spans="1:19">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" s="38" t="s">
         <v>87</v>
       </c>
@@ -8904,7 +8917,7 @@
       <c r="M95" s="24"/>
       <c r="N95" s="24"/>
     </row>
-    <row r="96" spans="1:19">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" s="40" t="s">
         <v>88</v>
       </c>
@@ -8948,7 +8961,7 @@
         <v>-9.581053715541632E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:14">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="49" t="s">
         <v>38</v>
       </c>
@@ -8992,7 +9005,7 @@
         <v>-5.7355997823842264</v>
       </c>
     </row>
-    <row r="98" spans="1:14">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="49" t="s">
         <v>39</v>
       </c>
@@ -9036,7 +9049,7 @@
         <v>-3.5654348703811789</v>
       </c>
     </row>
-    <row r="99" spans="1:14">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="49" t="s">
         <v>89</v>
       </c>
@@ -9080,7 +9093,7 @@
         <v>0.31873885819930781</v>
       </c>
     </row>
-    <row r="100" spans="1:14">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="49" t="s">
         <v>41</v>
       </c>
@@ -9124,7 +9137,7 @@
         <v>-1.2463893333830467</v>
       </c>
     </row>
-    <row r="101" spans="1:14">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="49" t="s">
         <v>90</v>
       </c>
@@ -9168,7 +9181,7 @@
         <v>1.036021818121502</v>
       </c>
     </row>
-    <row r="102" spans="1:14">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="40" t="s">
         <v>91</v>
       </c>
@@ -9212,7 +9225,7 @@
         <v>-1.0240600077349837</v>
       </c>
     </row>
-    <row r="103" spans="1:14">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="49" t="s">
         <v>38</v>
       </c>
@@ -9256,7 +9269,7 @@
         <v>-4.9019654919539191</v>
       </c>
     </row>
-    <row r="104" spans="1:14">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="49" t="s">
         <v>39</v>
       </c>
@@ -9300,7 +9313,7 @@
         <v>-1.2013597695918476</v>
       </c>
     </row>
-    <row r="105" spans="1:14">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="49" t="s">
         <v>89</v>
       </c>
@@ -9344,7 +9357,7 @@
         <v>-0.1536100133290752</v>
       </c>
     </row>
-    <row r="106" spans="1:14">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="49" t="s">
         <v>59</v>
       </c>
@@ -9388,7 +9401,7 @@
         <v>1.5797403375073849</v>
       </c>
     </row>
-    <row r="107" spans="1:14">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="49" t="s">
         <v>92</v>
       </c>
@@ -9432,7 +9445,7 @@
         <v>-8.4811639946390631</v>
       </c>
     </row>
-    <row r="108" spans="1:14">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="49" t="s">
         <v>65</v>
       </c>
@@ -9476,7 +9489,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="11.45">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="47" t="s">
         <v>93</v>
       </c>
@@ -9520,7 +9533,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="12" customHeight="1">
+    <row r="110" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="49"/>
       <c r="B110" s="49"/>
       <c r="C110" s="49"/>
@@ -9536,7 +9549,7 @@
       <c r="M110" s="23"/>
       <c r="N110" s="23"/>
     </row>
-    <row r="111" spans="1:14">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="38" t="s">
         <v>94</v>
       </c>
@@ -9554,7 +9567,7 @@
       <c r="M111" s="30"/>
       <c r="N111" s="30"/>
     </row>
-    <row r="112" spans="1:14" ht="11.45">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="47" t="s">
         <v>95</v>
       </c>
@@ -9598,7 +9611,7 @@
         <v>0.2796780289620715</v>
       </c>
     </row>
-    <row r="113" spans="1:14">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" s="49" t="s">
         <v>96</v>
       </c>
@@ -9642,7 +9655,7 @@
         <v>-1.0805630850672099</v>
       </c>
     </row>
-    <row r="114" spans="1:14">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="40" t="s">
         <v>97</v>
       </c>
@@ -9660,7 +9673,7 @@
       <c r="M114" s="23"/>
       <c r="N114" s="23"/>
     </row>
-    <row r="115" spans="1:14" ht="11.45">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="49" t="s">
         <v>98</v>
       </c>
@@ -9704,7 +9717,7 @@
         <v>-1.2228498427479972</v>
       </c>
     </row>
-    <row r="116" spans="1:14">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="62" t="s">
         <v>99</v>
       </c>
@@ -9748,7 +9761,7 @@
         <v>-1.4081959051479576</v>
       </c>
     </row>
-    <row r="117" spans="1:14">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" s="62" t="s">
         <v>100</v>
       </c>
@@ -9792,7 +9805,7 @@
         <v>-1.036664372257412</v>
       </c>
     </row>
-    <row r="118" spans="1:14">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" s="49" t="s">
         <v>101</v>
       </c>
@@ -9836,7 +9849,7 @@
         <v>-0.11695786118455231</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="11.45">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="49" t="s">
         <v>102</v>
       </c>
@@ -9880,7 +9893,7 @@
         <v>0.13339716097287013</v>
       </c>
     </row>
-    <row r="120" spans="1:14">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" s="40" t="s">
         <v>103</v>
       </c>
@@ -9898,7 +9911,7 @@
       <c r="M120" s="23"/>
       <c r="N120" s="23"/>
     </row>
-    <row r="121" spans="1:14">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" s="75" t="s">
         <v>104</v>
       </c>
@@ -9942,241 +9955,241 @@
         <v>-1.922623547071578</v>
       </c>
     </row>
-    <row r="122" spans="1:14" s="34" customFormat="1" ht="10.9">
-      <c r="A122" s="103" t="s">
+    <row r="122" spans="1:14" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
+      <c r="A122" s="105" t="s">
         <v>105</v>
       </c>
-      <c r="B122" s="104"/>
-      <c r="C122" s="104"/>
-      <c r="D122" s="104"/>
-      <c r="E122" s="104"/>
-      <c r="F122" s="104"/>
-      <c r="G122" s="104"/>
-      <c r="H122" s="104"/>
-      <c r="I122" s="104"/>
-      <c r="J122" s="104"/>
-      <c r="K122" s="104"/>
-      <c r="L122" s="104"/>
-      <c r="M122" s="104"/>
-      <c r="N122" s="104"/>
-    </row>
-    <row r="123" spans="1:14" s="34" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A123" s="101" t="s">
+      <c r="B122" s="106"/>
+      <c r="C122" s="106"/>
+      <c r="D122" s="106"/>
+      <c r="E122" s="106"/>
+      <c r="F122" s="106"/>
+      <c r="G122" s="106"/>
+      <c r="H122" s="106"/>
+      <c r="I122" s="106"/>
+      <c r="J122" s="106"/>
+      <c r="K122" s="106"/>
+      <c r="L122" s="106"/>
+      <c r="M122" s="106"/>
+      <c r="N122" s="106"/>
+    </row>
+    <row r="123" spans="1:14" s="34" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="103" t="s">
         <v>106</v>
       </c>
-      <c r="B123" s="101"/>
-      <c r="C123" s="101"/>
-      <c r="D123" s="101"/>
-      <c r="E123" s="101"/>
-      <c r="F123" s="101"/>
-      <c r="G123" s="101"/>
-      <c r="H123" s="101"/>
-      <c r="I123" s="101"/>
-      <c r="J123" s="101"/>
-      <c r="K123" s="101"/>
-      <c r="L123" s="101"/>
-      <c r="M123" s="101"/>
-      <c r="N123" s="101"/>
-    </row>
-    <row r="124" spans="1:14" s="34" customFormat="1" ht="10.9">
-      <c r="A124" s="101" t="s">
+      <c r="B123" s="103"/>
+      <c r="C123" s="103"/>
+      <c r="D123" s="103"/>
+      <c r="E123" s="103"/>
+      <c r="F123" s="103"/>
+      <c r="G123" s="103"/>
+      <c r="H123" s="103"/>
+      <c r="I123" s="103"/>
+      <c r="J123" s="103"/>
+      <c r="K123" s="103"/>
+      <c r="L123" s="103"/>
+      <c r="M123" s="103"/>
+      <c r="N123" s="103"/>
+    </row>
+    <row r="124" spans="1:14" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
+      <c r="A124" s="103" t="s">
         <v>107</v>
       </c>
-      <c r="B124" s="102"/>
-      <c r="C124" s="102"/>
-      <c r="D124" s="102"/>
-      <c r="E124" s="102"/>
-      <c r="F124" s="102"/>
-      <c r="G124" s="102"/>
-      <c r="H124" s="102"/>
-      <c r="I124" s="102"/>
-      <c r="J124" s="102"/>
-      <c r="K124" s="102"/>
-      <c r="L124" s="102"/>
-      <c r="M124" s="102"/>
-      <c r="N124" s="102"/>
-    </row>
-    <row r="125" spans="1:14" s="34" customFormat="1" ht="10.9">
-      <c r="A125" s="101" t="s">
+      <c r="B124" s="104"/>
+      <c r="C124" s="104"/>
+      <c r="D124" s="104"/>
+      <c r="E124" s="104"/>
+      <c r="F124" s="104"/>
+      <c r="G124" s="104"/>
+      <c r="H124" s="104"/>
+      <c r="I124" s="104"/>
+      <c r="J124" s="104"/>
+      <c r="K124" s="104"/>
+      <c r="L124" s="104"/>
+      <c r="M124" s="104"/>
+      <c r="N124" s="104"/>
+    </row>
+    <row r="125" spans="1:14" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
+      <c r="A125" s="103" t="s">
         <v>108</v>
       </c>
-      <c r="B125" s="102"/>
-      <c r="C125" s="102"/>
-      <c r="D125" s="102"/>
-      <c r="E125" s="102"/>
-      <c r="F125" s="102"/>
-      <c r="G125" s="102"/>
-      <c r="H125" s="102"/>
-      <c r="I125" s="102"/>
-      <c r="J125" s="102"/>
-      <c r="K125" s="102"/>
-      <c r="L125" s="102"/>
-      <c r="M125" s="102"/>
-      <c r="N125" s="102"/>
-    </row>
-    <row r="126" spans="1:14" s="34" customFormat="1" ht="10.9">
-      <c r="A126" s="101" t="s">
+      <c r="B125" s="104"/>
+      <c r="C125" s="104"/>
+      <c r="D125" s="104"/>
+      <c r="E125" s="104"/>
+      <c r="F125" s="104"/>
+      <c r="G125" s="104"/>
+      <c r="H125" s="104"/>
+      <c r="I125" s="104"/>
+      <c r="J125" s="104"/>
+      <c r="K125" s="104"/>
+      <c r="L125" s="104"/>
+      <c r="M125" s="104"/>
+      <c r="N125" s="104"/>
+    </row>
+    <row r="126" spans="1:14" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
+      <c r="A126" s="103" t="s">
         <v>109</v>
       </c>
-      <c r="B126" s="102"/>
-      <c r="C126" s="102"/>
-      <c r="D126" s="102"/>
-      <c r="E126" s="102"/>
-      <c r="F126" s="102"/>
-      <c r="G126" s="102"/>
-      <c r="H126" s="102"/>
-      <c r="I126" s="102"/>
-      <c r="J126" s="102"/>
-      <c r="K126" s="102"/>
-      <c r="L126" s="102"/>
-      <c r="M126" s="102"/>
-      <c r="N126" s="102"/>
-    </row>
-    <row r="127" spans="1:14" s="34" customFormat="1" ht="10.9">
-      <c r="A127" s="101" t="s">
+      <c r="B126" s="104"/>
+      <c r="C126" s="104"/>
+      <c r="D126" s="104"/>
+      <c r="E126" s="104"/>
+      <c r="F126" s="104"/>
+      <c r="G126" s="104"/>
+      <c r="H126" s="104"/>
+      <c r="I126" s="104"/>
+      <c r="J126" s="104"/>
+      <c r="K126" s="104"/>
+      <c r="L126" s="104"/>
+      <c r="M126" s="104"/>
+      <c r="N126" s="104"/>
+    </row>
+    <row r="127" spans="1:14" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
+      <c r="A127" s="103" t="s">
         <v>110</v>
       </c>
-      <c r="B127" s="102"/>
-      <c r="C127" s="102"/>
-      <c r="D127" s="102"/>
-      <c r="E127" s="102"/>
-      <c r="F127" s="102"/>
-      <c r="G127" s="102"/>
-      <c r="H127" s="102"/>
-      <c r="I127" s="102"/>
-      <c r="J127" s="102"/>
-      <c r="K127" s="102"/>
-      <c r="L127" s="102"/>
-      <c r="M127" s="102"/>
-      <c r="N127" s="102"/>
-    </row>
-    <row r="128" spans="1:14" s="34" customFormat="1" ht="10.9">
-      <c r="A128" s="101" t="s">
+      <c r="B127" s="104"/>
+      <c r="C127" s="104"/>
+      <c r="D127" s="104"/>
+      <c r="E127" s="104"/>
+      <c r="F127" s="104"/>
+      <c r="G127" s="104"/>
+      <c r="H127" s="104"/>
+      <c r="I127" s="104"/>
+      <c r="J127" s="104"/>
+      <c r="K127" s="104"/>
+      <c r="L127" s="104"/>
+      <c r="M127" s="104"/>
+      <c r="N127" s="104"/>
+    </row>
+    <row r="128" spans="1:14" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
+      <c r="A128" s="103" t="s">
         <v>111</v>
       </c>
-      <c r="B128" s="102"/>
-      <c r="C128" s="102"/>
-      <c r="D128" s="102"/>
-      <c r="E128" s="102"/>
-      <c r="F128" s="102"/>
-      <c r="G128" s="102"/>
-      <c r="H128" s="102"/>
-      <c r="I128" s="102"/>
-      <c r="J128" s="102"/>
-      <c r="K128" s="102"/>
-      <c r="L128" s="102"/>
-      <c r="M128" s="102"/>
-      <c r="N128" s="102"/>
-    </row>
-    <row r="129" spans="1:14" s="34" customFormat="1" ht="10.9">
-      <c r="A129" s="101" t="s">
+      <c r="B128" s="104"/>
+      <c r="C128" s="104"/>
+      <c r="D128" s="104"/>
+      <c r="E128" s="104"/>
+      <c r="F128" s="104"/>
+      <c r="G128" s="104"/>
+      <c r="H128" s="104"/>
+      <c r="I128" s="104"/>
+      <c r="J128" s="104"/>
+      <c r="K128" s="104"/>
+      <c r="L128" s="104"/>
+      <c r="M128" s="104"/>
+      <c r="N128" s="104"/>
+    </row>
+    <row r="129" spans="1:14" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
+      <c r="A129" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="B129" s="102"/>
-      <c r="C129" s="102"/>
-      <c r="D129" s="102"/>
-      <c r="E129" s="102"/>
-      <c r="F129" s="102"/>
-      <c r="G129" s="102"/>
-      <c r="H129" s="102"/>
-      <c r="I129" s="102"/>
-      <c r="J129" s="102"/>
-      <c r="K129" s="102"/>
-      <c r="L129" s="102"/>
-      <c r="M129" s="102"/>
-      <c r="N129" s="102"/>
-    </row>
-    <row r="130" spans="1:14" s="34" customFormat="1" ht="10.9">
-      <c r="A130" s="101" t="s">
+      <c r="B129" s="104"/>
+      <c r="C129" s="104"/>
+      <c r="D129" s="104"/>
+      <c r="E129" s="104"/>
+      <c r="F129" s="104"/>
+      <c r="G129" s="104"/>
+      <c r="H129" s="104"/>
+      <c r="I129" s="104"/>
+      <c r="J129" s="104"/>
+      <c r="K129" s="104"/>
+      <c r="L129" s="104"/>
+      <c r="M129" s="104"/>
+      <c r="N129" s="104"/>
+    </row>
+    <row r="130" spans="1:14" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
+      <c r="A130" s="103" t="s">
         <v>113</v>
       </c>
-      <c r="B130" s="102"/>
-      <c r="C130" s="102"/>
-      <c r="D130" s="102"/>
-      <c r="E130" s="102"/>
-      <c r="F130" s="102"/>
-      <c r="G130" s="102"/>
-      <c r="H130" s="102"/>
-      <c r="I130" s="102"/>
-      <c r="J130" s="102"/>
-      <c r="K130" s="102"/>
-      <c r="L130" s="102"/>
-      <c r="M130" s="102"/>
-      <c r="N130" s="102"/>
-    </row>
-    <row r="131" spans="1:14" s="34" customFormat="1" ht="10.9">
-      <c r="A131" s="101" t="s">
+      <c r="B130" s="104"/>
+      <c r="C130" s="104"/>
+      <c r="D130" s="104"/>
+      <c r="E130" s="104"/>
+      <c r="F130" s="104"/>
+      <c r="G130" s="104"/>
+      <c r="H130" s="104"/>
+      <c r="I130" s="104"/>
+      <c r="J130" s="104"/>
+      <c r="K130" s="104"/>
+      <c r="L130" s="104"/>
+      <c r="M130" s="104"/>
+      <c r="N130" s="104"/>
+    </row>
+    <row r="131" spans="1:14" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
+      <c r="A131" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="B131" s="102"/>
-      <c r="C131" s="102"/>
-      <c r="D131" s="102"/>
-      <c r="E131" s="102"/>
-      <c r="F131" s="102"/>
-      <c r="G131" s="102"/>
-      <c r="H131" s="102"/>
-      <c r="I131" s="102"/>
-      <c r="J131" s="102"/>
-      <c r="K131" s="102"/>
-      <c r="L131" s="102"/>
-      <c r="M131" s="102"/>
-      <c r="N131" s="102"/>
-    </row>
-    <row r="132" spans="1:14" s="34" customFormat="1" ht="10.9">
-      <c r="A132" s="101" t="s">
+      <c r="B131" s="104"/>
+      <c r="C131" s="104"/>
+      <c r="D131" s="104"/>
+      <c r="E131" s="104"/>
+      <c r="F131" s="104"/>
+      <c r="G131" s="104"/>
+      <c r="H131" s="104"/>
+      <c r="I131" s="104"/>
+      <c r="J131" s="104"/>
+      <c r="K131" s="104"/>
+      <c r="L131" s="104"/>
+      <c r="M131" s="104"/>
+      <c r="N131" s="104"/>
+    </row>
+    <row r="132" spans="1:14" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
+      <c r="A132" s="103" t="s">
         <v>115</v>
       </c>
-      <c r="B132" s="102"/>
-      <c r="C132" s="102"/>
-      <c r="D132" s="102"/>
-      <c r="E132" s="102"/>
-      <c r="F132" s="102"/>
-      <c r="G132" s="102"/>
-      <c r="H132" s="102"/>
-      <c r="I132" s="102"/>
-      <c r="J132" s="102"/>
-      <c r="K132" s="102"/>
-      <c r="L132" s="102"/>
-      <c r="M132" s="102"/>
-      <c r="N132" s="102"/>
-    </row>
-    <row r="133" spans="1:14" s="34" customFormat="1" ht="10.9">
-      <c r="A133" s="101" t="s">
+      <c r="B132" s="104"/>
+      <c r="C132" s="104"/>
+      <c r="D132" s="104"/>
+      <c r="E132" s="104"/>
+      <c r="F132" s="104"/>
+      <c r="G132" s="104"/>
+      <c r="H132" s="104"/>
+      <c r="I132" s="104"/>
+      <c r="J132" s="104"/>
+      <c r="K132" s="104"/>
+      <c r="L132" s="104"/>
+      <c r="M132" s="104"/>
+      <c r="N132" s="104"/>
+    </row>
+    <row r="133" spans="1:14" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
+      <c r="A133" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="B133" s="102"/>
-      <c r="C133" s="102"/>
-      <c r="D133" s="102"/>
-      <c r="E133" s="102"/>
-      <c r="F133" s="102"/>
-      <c r="G133" s="102"/>
-      <c r="H133" s="102"/>
-      <c r="I133" s="102"/>
-      <c r="J133" s="102"/>
-      <c r="K133" s="102"/>
-      <c r="L133" s="102"/>
-      <c r="M133" s="102"/>
-      <c r="N133" s="102"/>
-    </row>
-    <row r="134" spans="1:14" s="34" customFormat="1" ht="11.45" thickBot="1">
-      <c r="A134" s="105" t="s">
+      <c r="B133" s="104"/>
+      <c r="C133" s="104"/>
+      <c r="D133" s="104"/>
+      <c r="E133" s="104"/>
+      <c r="F133" s="104"/>
+      <c r="G133" s="104"/>
+      <c r="H133" s="104"/>
+      <c r="I133" s="104"/>
+      <c r="J133" s="104"/>
+      <c r="K133" s="104"/>
+      <c r="L133" s="104"/>
+      <c r="M133" s="104"/>
+      <c r="N133" s="104"/>
+    </row>
+    <row r="134" spans="1:14" s="34" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="101" t="s">
         <v>117</v>
       </c>
-      <c r="B134" s="106"/>
-      <c r="C134" s="106"/>
-      <c r="D134" s="106"/>
-      <c r="E134" s="106"/>
-      <c r="F134" s="106"/>
-      <c r="G134" s="106"/>
-      <c r="H134" s="106"/>
-      <c r="I134" s="106"/>
-      <c r="J134" s="106"/>
-      <c r="K134" s="106"/>
-      <c r="L134" s="106"/>
-      <c r="M134" s="106"/>
-      <c r="N134" s="106"/>
-    </row>
-    <row r="135" spans="1:14">
+      <c r="B134" s="102"/>
+      <c r="C134" s="102"/>
+      <c r="D134" s="102"/>
+      <c r="E134" s="102"/>
+      <c r="F134" s="102"/>
+      <c r="G134" s="102"/>
+      <c r="H134" s="102"/>
+      <c r="I134" s="102"/>
+      <c r="J134" s="102"/>
+      <c r="K134" s="102"/>
+      <c r="L134" s="102"/>
+      <c r="M134" s="102"/>
+      <c r="N134" s="102"/>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="35" t="s">
         <v>118</v>
       </c>
@@ -10193,6 +10206,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A127:N127"/>
+    <mergeCell ref="A122:N122"/>
+    <mergeCell ref="A123:N123"/>
+    <mergeCell ref="A124:N124"/>
+    <mergeCell ref="A125:N125"/>
+    <mergeCell ref="A126:N126"/>
     <mergeCell ref="A134:N134"/>
     <mergeCell ref="A128:N128"/>
     <mergeCell ref="A129:N129"/>
@@ -10200,12 +10219,6 @@
     <mergeCell ref="A131:N131"/>
     <mergeCell ref="A132:N132"/>
     <mergeCell ref="A133:N133"/>
-    <mergeCell ref="A127:N127"/>
-    <mergeCell ref="A122:N122"/>
-    <mergeCell ref="A123:N123"/>
-    <mergeCell ref="A124:N124"/>
-    <mergeCell ref="A125:N125"/>
-    <mergeCell ref="A126:N126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10216,21 +10229,21 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="82" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1"/>
-    <row r="3" spans="1:2" ht="15" thickBot="1">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="83" t="s">
         <v>120</v>
       </c>
@@ -10238,7 +10251,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -10246,7 +10259,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -10254,7 +10267,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -10275,11 +10288,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85806999-68DD-4706-A5C4-8DE674DA542A}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
@@ -10287,7 +10300,7 @@
     <col min="5" max="5" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
         <v>124</v>
       </c>
@@ -10303,7 +10316,7 @@
       <c r="K1" s="108"/>
       <c r="L1" s="108"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="107" t="s">
@@ -10322,7 +10335,7 @@
       <c r="J3" s="107"/>
       <c r="K3" s="107"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9" t="s">
         <v>128</v>
@@ -10355,7 +10368,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>129</v>
       </c>
@@ -10386,7 +10399,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>130</v>
       </c>
@@ -10417,7 +10430,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>131</v>
       </c>
@@ -10448,7 +10461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>132</v>
       </c>
@@ -10479,7 +10492,7 @@
         <v>138.37484564921732</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>133</v>
       </c>
@@ -10514,7 +10527,7 @@
         <v>1391.2172148280033</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>134</v>
       </c>
@@ -10545,7 +10558,7 @@
         <v>35.20825</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>135</v>
       </c>
@@ -10576,7 +10589,7 @@
         <v>28.571428571428573</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>136</v>
       </c>
@@ -10611,7 +10624,7 @@
         <v>22.988256601844338</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>137</v>
       </c>
@@ -10632,11 +10645,11 @@
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H14" s="11"/>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>126</v>
       </c>
@@ -10653,7 +10666,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>138</v>
       </c>
@@ -10674,7 +10687,7 @@
         <v>1407.4461100019494</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>139</v>
       </c>
@@ -10695,7 +10708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -10716,7 +10729,7 @@
         <v>0.98478601926509657</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>141</v>
       </c>
@@ -10737,7 +10750,7 @@
         <v>1.5213980734903397E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>142</v>
       </c>
@@ -10758,8 +10771,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1"/>
-    <row r="22" spans="1:5">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>143</v>
       </c>
@@ -10776,7 +10789,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>144</v>
       </c>
@@ -10797,7 +10810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>145</v>
       </c>
@@ -10818,7 +10831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>146</v>
       </c>
@@ -10839,15 +10852,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1">
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="90"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="97" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="48" spans="2:2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="97" t="s">
         <v>148</v>
       </c>
@@ -10866,18 +10879,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DB41427-AB65-4280-A83C-90CCC833C195}">
-  <dimension ref="A1:AF14"/>
+  <dimension ref="A1:AF16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>149</v>
       </c>
@@ -10975,7 +10988,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>150</v>
       </c>
@@ -11104,7 +11117,7 @@
         <v>0.16555189491787298</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>151</v>
       </c>
@@ -11233,7 +11246,7 @@
         <v>0.62632340757933302</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>152</v>
       </c>
@@ -11331,7 +11344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>153</v>
       </c>
@@ -11429,7 +11442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>154</v>
       </c>
@@ -11527,7 +11540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>155</v>
       </c>
@@ -11656,7 +11669,7 @@
         <v>0.20812469750279411</v>
       </c>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>156</v>
       </c>
@@ -11785,19 +11798,24 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B12" s="87" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B13" s="92" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B14" s="91" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B16" s="109" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -11810,18 +11828,18 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:AF16"/>
+  <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>149</v>
       </c>
@@ -11919,652 +11937,652 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>150</v>
       </c>
       <c r="B2" s="99">
-        <f>Calculations!B2</f>
-        <v>3.9941983335235649E-5</v>
+        <f>Calculations!B2/SUM(Calculations!B$2:B$6)</f>
+        <v>5.3213834166182343E-5</v>
       </c>
       <c r="C2" s="99">
-        <f>Calculations!C2</f>
-        <v>5.1644186997708698E-4</v>
+        <f>Calculations!C2/SUM(Calculations!C$2:C$6)</f>
+        <v>6.8793532593692858E-4</v>
       </c>
       <c r="D2" s="99">
-        <f>Calculations!D2</f>
-        <v>9.929417566189383E-4</v>
+        <f>Calculations!D2/SUM(Calculations!D$2:D$6)</f>
+        <v>1.3224558817292863E-3</v>
       </c>
       <c r="E2" s="99">
-        <f>Calculations!E2</f>
-        <v>1.4694416432607898E-3</v>
+        <f>Calculations!E2/SUM(Calculations!E$2:E$6)</f>
+        <v>1.9567755969446513E-3</v>
       </c>
       <c r="F2" s="99">
-        <f>Calculations!F2</f>
-        <v>1.9459415299026412E-3</v>
+        <f>Calculations!F2/SUM(Calculations!F$2:F$6)</f>
+        <v>2.5908945669240349E-3</v>
       </c>
       <c r="G2" s="99">
-        <f>Calculations!G2</f>
-        <v>2.4224414165444925E-3</v>
+        <f>Calculations!G2/SUM(Calculations!G$2:G$6)</f>
+        <v>3.2248128869481136E-3</v>
       </c>
       <c r="H2" s="99">
-        <f>Calculations!H2</f>
-        <v>2.898941303186344E-3</v>
+        <f>Calculations!H2/SUM(Calculations!H$2:H$6)</f>
+        <v>3.8585306522372744E-3</v>
       </c>
       <c r="I2" s="99">
-        <f>Calculations!I2</f>
-        <v>3.3754411898281951E-3</v>
+        <f>Calculations!I2/SUM(Calculations!I$2:I$6)</f>
+        <v>4.4920479579516632E-3</v>
       </c>
       <c r="J2" s="99">
-        <f>Calculations!J2</f>
-        <v>3.8519410764700467E-3</v>
+        <f>Calculations!J2/SUM(Calculations!J$2:J$6)</f>
+        <v>5.1253648991912339E-3</v>
       </c>
       <c r="K2" s="99">
-        <f>Calculations!K2</f>
-        <v>4.3284409631118978E-3</v>
+        <f>Calculations!K2/SUM(Calculations!K$2:K$6)</f>
+        <v>5.7584815709957942E-3</v>
       </c>
       <c r="L2" s="99">
-        <f>Calculations!L2</f>
-        <v>4.8049408497537489E-3</v>
+        <f>Calculations!L2/SUM(Calculations!L$2:L$6)</f>
+        <v>6.3913980683450514E-3</v>
       </c>
       <c r="M2" s="99">
-        <f>Calculations!M2</f>
-        <v>1.2232538513214927E-2</v>
+        <f>Calculations!M2/SUM(Calculations!M$2:M$6)</f>
+        <v>1.6231383162068E-2</v>
       </c>
       <c r="N2" s="99">
-        <f>Calculations!N2</f>
-        <v>1.9660136176676106E-2</v>
+        <f>Calculations!N2/SUM(Calculations!N$2:N$6)</f>
+        <v>2.6023110205325765E-2</v>
       </c>
       <c r="O2" s="99">
-        <f>Calculations!O2</f>
-        <v>2.7087733840137282E-2</v>
+        <f>Calculations!O2/SUM(Calculations!O$2:O$6)</f>
+        <v>3.576693333627104E-2</v>
       </c>
       <c r="P2" s="99">
-        <f>Calculations!P2</f>
-        <v>3.4515331503598465E-2</v>
+        <f>Calculations!P2/SUM(Calculations!P$2:P$6)</f>
+        <v>4.546320323642291E-2</v>
       </c>
       <c r="Q2" s="99">
-        <f>Calculations!Q2</f>
-        <v>4.1942929167059641E-2</v>
+        <f>Calculations!Q2/SUM(Calculations!Q$2:Q$6)</f>
+        <v>5.5112267172738066E-2</v>
       </c>
       <c r="R2" s="99">
-        <f>Calculations!R2</f>
-        <v>4.9370526830520817E-2</v>
+        <f>Calculations!R2/SUM(Calculations!R$2:R$6)</f>
+        <v>6.4714469039069161E-2</v>
       </c>
       <c r="S2" s="99">
-        <f>Calculations!S2</f>
-        <v>5.6798124493982E-2</v>
+        <f>Calculations!S2/SUM(Calculations!S$2:S$6)</f>
+        <v>7.4270149397020507E-2</v>
       </c>
       <c r="T2" s="99">
-        <f>Calculations!T2</f>
-        <v>6.4225722157443182E-2</v>
+        <f>Calculations!T2/SUM(Calculations!T$2:T$6)</f>
+        <v>8.3779645516211296E-2</v>
       </c>
       <c r="U2" s="99">
-        <f>Calculations!U2</f>
-        <v>7.1653319820904351E-2</v>
+        <f>Calculations!U2/SUM(Calculations!U$2:U$6)</f>
+        <v>9.3243291413956611E-2</v>
       </c>
       <c r="V2" s="99">
-        <f>Calculations!V2</f>
-        <v>7.9080917484365534E-2</v>
+        <f>Calculations!V2/SUM(Calculations!V$2:V$6)</f>
+        <v>0.10266141789437581</v>
       </c>
       <c r="W2" s="99">
-        <f>Calculations!W2</f>
-        <v>8.7728015227716283E-2</v>
+        <f>Calculations!W2/SUM(Calculations!W$2:W$6)</f>
+        <v>0.1135689512148802</v>
       </c>
       <c r="X2" s="99">
-        <f>Calculations!X2</f>
-        <v>9.6375112971067017E-2</v>
+        <f>Calculations!X2/SUM(Calculations!X$2:X$6)</f>
+        <v>0.12441574637303589</v>
       </c>
       <c r="Y2" s="99">
-        <f>Calculations!Y2</f>
-        <v>0.10502221071441777</v>
+        <f>Calculations!Y2/SUM(Calculations!Y$2:Y$6)</f>
+        <v>0.13520230928728549</v>
       </c>
       <c r="Z2" s="99">
-        <f>Calculations!Z2</f>
-        <v>0.11366930845776851</v>
+        <f>Calculations!Z2/SUM(Calculations!Z$2:Z$6)</f>
+        <v>0.14592914027289947</v>
       </c>
       <c r="AA2" s="99">
-        <f>Calculations!AA2</f>
-        <v>0.12231640620111926</v>
+        <f>Calculations!AA2/SUM(Calculations!AA$2:AA$6)</f>
+        <v>0.15659673411933259</v>
       </c>
       <c r="AB2" s="99">
-        <f>Calculations!AB2</f>
-        <v>0.13096350394447001</v>
+        <f>Calculations!AB2/SUM(Calculations!AB$2:AB$6)</f>
+        <v>0.16720558016630246</v>
       </c>
       <c r="AC2" s="99">
-        <f>Calculations!AC2</f>
-        <v>0.13961060168782075</v>
+        <f>Calculations!AC2/SUM(Calculations!AC$2:AC$6)</f>
+        <v>0.17775616237861439</v>
       </c>
       <c r="AD2" s="99">
-        <f>Calculations!AD2</f>
-        <v>0.14825769943117151</v>
+        <f>Calculations!AD2/SUM(Calculations!AD$2:AD$6)</f>
+        <v>0.18824895941975692</v>
       </c>
       <c r="AE2" s="99">
-        <f>Calculations!AE2</f>
-        <v>0.15690479717452224</v>
+        <f>Calculations!AE2/SUM(Calculations!AE$2:AE$6)</f>
+        <v>0.19868444472429142</v>
       </c>
       <c r="AF2" s="99">
-        <f>Calculations!AF2</f>
-        <v>0.16555189491787298</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32">
+        <f>Calculations!AF2/SUM(Calculations!AF$2:AF$6)</f>
+        <v>0.20906308656905875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>151</v>
       </c>
       <c r="B3" s="99">
-        <f>Calculations!B3</f>
-        <v>0.75055403345734029</v>
+        <f>Calculations!B3/SUM(Calculations!B$2:B$6)</f>
+        <v>0.99994678616583377</v>
       </c>
       <c r="C3" s="99">
-        <f>Calculations!C3</f>
-        <v>0.75019638026010127</v>
+        <f>Calculations!C3/SUM(Calculations!C$2:C$6)</f>
+        <v>0.99931206467406297</v>
       </c>
       <c r="D3" s="99">
-        <f>Calculations!D3</f>
-        <v>0.74983872706286214</v>
+        <f>Calculations!D3/SUM(Calculations!D$2:D$6)</f>
+        <v>0.99867754411827081</v>
       </c>
       <c r="E3" s="99">
-        <f>Calculations!E3</f>
-        <v>0.74948107386562313</v>
+        <f>Calculations!E3/SUM(Calculations!E$2:E$6)</f>
+        <v>0.99804322440305537</v>
       </c>
       <c r="F3" s="99">
-        <f>Calculations!F3</f>
-        <v>0.749123420668384</v>
+        <f>Calculations!F3/SUM(Calculations!F$2:F$6)</f>
+        <v>0.99740910543307593</v>
       </c>
       <c r="G3" s="99">
-        <f>Calculations!G3</f>
-        <v>0.74876576747114498</v>
+        <f>Calculations!G3/SUM(Calculations!G$2:G$6)</f>
+        <v>0.99677518711305191</v>
       </c>
       <c r="H3" s="99">
-        <f>Calculations!H3</f>
-        <v>0.74840811427390597</v>
+        <f>Calculations!H3/SUM(Calculations!H$2:H$6)</f>
+        <v>0.99614146934776271</v>
       </c>
       <c r="I3" s="99">
-        <f>Calculations!I3</f>
-        <v>0.74805046107666684</v>
+        <f>Calculations!I3/SUM(Calculations!I$2:I$6)</f>
+        <v>0.99550795204204823</v>
       </c>
       <c r="J3" s="99">
-        <f>Calculations!J3</f>
-        <v>0.74769280787942782</v>
+        <f>Calculations!J3/SUM(Calculations!J$2:J$6)</f>
+        <v>0.99487463510080876</v>
       </c>
       <c r="K3" s="99">
-        <f>Calculations!K3</f>
-        <v>0.7473351546821887</v>
+        <f>Calculations!K3/SUM(Calculations!K$2:K$6)</f>
+        <v>0.99424151842900421</v>
       </c>
       <c r="L3" s="99">
-        <f>Calculations!L3</f>
-        <v>0.74697750148494968</v>
+        <f>Calculations!L3/SUM(Calculations!L$2:L$6)</f>
+        <v>0.9936086019316549</v>
       </c>
       <c r="M3" s="99">
-        <f>Calculations!M3</f>
-        <v>0.74140246542174304</v>
+        <f>Calculations!M3/SUM(Calculations!M$2:M$6)</f>
+        <v>0.98376861683793204</v>
       </c>
       <c r="N3" s="99">
-        <f>Calculations!N3</f>
-        <v>0.7358274293585364</v>
+        <f>Calculations!N3/SUM(Calculations!N$2:N$6)</f>
+        <v>0.97397688979467434</v>
       </c>
       <c r="O3" s="99">
-        <f>Calculations!O3</f>
-        <v>0.73025239329532976</v>
+        <f>Calculations!O3/SUM(Calculations!O$2:O$6)</f>
+        <v>0.96423306666372899</v>
       </c>
       <c r="P3" s="99">
-        <f>Calculations!P3</f>
-        <v>0.72467735723212312</v>
+        <f>Calculations!P3/SUM(Calculations!P$2:P$6)</f>
+        <v>0.95453679676357717</v>
       </c>
       <c r="Q3" s="99">
-        <f>Calculations!Q3</f>
-        <v>0.71910232116891648</v>
+        <f>Calculations!Q3/SUM(Calculations!Q$2:Q$6)</f>
+        <v>0.94488773282726191</v>
       </c>
       <c r="R3" s="99">
-        <f>Calculations!R3</f>
-        <v>0.71352728510570995</v>
+        <f>Calculations!R3/SUM(Calculations!R$2:R$6)</f>
+        <v>0.93528553096093092</v>
       </c>
       <c r="S3" s="99">
-        <f>Calculations!S3</f>
-        <v>0.70795224904250331</v>
+        <f>Calculations!S3/SUM(Calculations!S$2:S$6)</f>
+        <v>0.92572985060297941</v>
       </c>
       <c r="T3" s="99">
-        <f>Calculations!T3</f>
-        <v>0.70237721297929667</v>
+        <f>Calculations!T3/SUM(Calculations!T$2:T$6)</f>
+        <v>0.91622035448378869</v>
       </c>
       <c r="U3" s="99">
-        <f>Calculations!U3</f>
-        <v>0.69680217691609003</v>
+        <f>Calculations!U3/SUM(Calculations!U$2:U$6)</f>
+        <v>0.90675670858604329</v>
       </c>
       <c r="V3" s="99">
-        <f>Calculations!V3</f>
-        <v>0.69122714085288339</v>
+        <f>Calculations!V3/SUM(Calculations!V$2:V$6)</f>
+        <v>0.89733858210562423</v>
       </c>
       <c r="W3" s="99">
-        <f>Calculations!W3</f>
-        <v>0.68473676752552837</v>
+        <f>Calculations!W3/SUM(Calculations!W$2:W$6)</f>
+        <v>0.88643104878511969</v>
       </c>
       <c r="X3" s="99">
-        <f>Calculations!X3</f>
-        <v>0.67824639419817334</v>
+        <f>Calculations!X3/SUM(Calculations!X$2:X$6)</f>
+        <v>0.87558425362696402</v>
       </c>
       <c r="Y3" s="99">
-        <f>Calculations!Y3</f>
-        <v>0.67175602087081832</v>
+        <f>Calculations!Y3/SUM(Calculations!Y$2:Y$6)</f>
+        <v>0.86479769071271451</v>
       </c>
       <c r="Z3" s="99">
-        <f>Calculations!Z3</f>
-        <v>0.66526564754346329</v>
+        <f>Calculations!Z3/SUM(Calculations!Z$2:Z$6)</f>
+        <v>0.85407085972710062</v>
       </c>
       <c r="AA3" s="99">
-        <f>Calculations!AA3</f>
-        <v>0.65877527421610815</v>
+        <f>Calculations!AA3/SUM(Calculations!AA$2:AA$6)</f>
+        <v>0.84340326588066739</v>
       </c>
       <c r="AB3" s="99">
-        <f>Calculations!AB3</f>
-        <v>0.65228490088875313</v>
+        <f>Calculations!AB3/SUM(Calculations!AB$2:AB$6)</f>
+        <v>0.83279441983369762</v>
       </c>
       <c r="AC3" s="99">
-        <f>Calculations!AC3</f>
-        <v>0.6457945275613981</v>
+        <f>Calculations!AC3/SUM(Calculations!AC$2:AC$6)</f>
+        <v>0.82224383762138564</v>
       </c>
       <c r="AD3" s="99">
-        <f>Calculations!AD3</f>
-        <v>0.63930415423404308</v>
+        <f>Calculations!AD3/SUM(Calculations!AD$2:AD$6)</f>
+        <v>0.81175104058024306</v>
       </c>
       <c r="AE3" s="99">
-        <f>Calculations!AE3</f>
-        <v>0.63281378090668805</v>
+        <f>Calculations!AE3/SUM(Calculations!AE$2:AE$6)</f>
+        <v>0.80131555527570864</v>
       </c>
       <c r="AF3" s="99">
-        <f>Calculations!AF3</f>
-        <v>0.62632340757933302</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32">
+        <f>Calculations!AF3/SUM(Calculations!AF$2:AF$6)</f>
+        <v>0.79093691343094119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>152</v>
       </c>
       <c r="B4" s="99">
-        <f>Calculations!B4</f>
+        <f>Calculations!B4/SUM(Calculations!B$2:B$6)</f>
         <v>0</v>
       </c>
       <c r="C4" s="99">
-        <f>Calculations!C4</f>
+        <f>Calculations!C4/SUM(Calculations!C$2:C$6)</f>
         <v>0</v>
       </c>
       <c r="D4" s="99">
-        <f>Calculations!D4</f>
+        <f>Calculations!D4/SUM(Calculations!D$2:D$6)</f>
         <v>0</v>
       </c>
       <c r="E4" s="99">
-        <f>Calculations!E4</f>
+        <f>Calculations!E4/SUM(Calculations!E$2:E$6)</f>
         <v>0</v>
       </c>
       <c r="F4" s="99">
-        <f>Calculations!F4</f>
+        <f>Calculations!F4/SUM(Calculations!F$2:F$6)</f>
         <v>0</v>
       </c>
       <c r="G4" s="99">
-        <f>Calculations!G4</f>
+        <f>Calculations!G4/SUM(Calculations!G$2:G$6)</f>
         <v>0</v>
       </c>
       <c r="H4" s="99">
-        <f>Calculations!H4</f>
+        <f>Calculations!H4/SUM(Calculations!H$2:H$6)</f>
         <v>0</v>
       </c>
       <c r="I4" s="99">
-        <f>Calculations!I4</f>
+        <f>Calculations!I4/SUM(Calculations!I$2:I$6)</f>
         <v>0</v>
       </c>
       <c r="J4" s="99">
-        <f>Calculations!J4</f>
+        <f>Calculations!J4/SUM(Calculations!J$2:J$6)</f>
         <v>0</v>
       </c>
       <c r="K4" s="99">
-        <f>Calculations!K4</f>
+        <f>Calculations!K4/SUM(Calculations!K$2:K$6)</f>
         <v>0</v>
       </c>
       <c r="L4" s="99">
-        <f>Calculations!L4</f>
+        <f>Calculations!L4/SUM(Calculations!L$2:L$6)</f>
         <v>0</v>
       </c>
       <c r="M4" s="99">
-        <f>Calculations!M4</f>
+        <f>Calculations!M4/SUM(Calculations!M$2:M$6)</f>
         <v>0</v>
       </c>
       <c r="N4" s="99">
-        <f>Calculations!N4</f>
+        <f>Calculations!N4/SUM(Calculations!N$2:N$6)</f>
         <v>0</v>
       </c>
       <c r="O4" s="99">
-        <f>Calculations!O4</f>
+        <f>Calculations!O4/SUM(Calculations!O$2:O$6)</f>
         <v>0</v>
       </c>
       <c r="P4" s="99">
-        <f>Calculations!P4</f>
+        <f>Calculations!P4/SUM(Calculations!P$2:P$6)</f>
         <v>0</v>
       </c>
       <c r="Q4" s="99">
-        <f>Calculations!Q4</f>
+        <f>Calculations!Q4/SUM(Calculations!Q$2:Q$6)</f>
         <v>0</v>
       </c>
       <c r="R4" s="99">
-        <f>Calculations!R4</f>
+        <f>Calculations!R4/SUM(Calculations!R$2:R$6)</f>
         <v>0</v>
       </c>
       <c r="S4" s="99">
-        <f>Calculations!S4</f>
+        <f>Calculations!S4/SUM(Calculations!S$2:S$6)</f>
         <v>0</v>
       </c>
       <c r="T4" s="99">
-        <f>Calculations!T4</f>
+        <f>Calculations!T4/SUM(Calculations!T$2:T$6)</f>
         <v>0</v>
       </c>
       <c r="U4" s="99">
-        <f>Calculations!U4</f>
+        <f>Calculations!U4/SUM(Calculations!U$2:U$6)</f>
         <v>0</v>
       </c>
       <c r="V4" s="99">
-        <f>Calculations!V4</f>
+        <f>Calculations!V4/SUM(Calculations!V$2:V$6)</f>
         <v>0</v>
       </c>
       <c r="W4" s="99">
-        <f>Calculations!W4</f>
+        <f>Calculations!W4/SUM(Calculations!W$2:W$6)</f>
         <v>0</v>
       </c>
       <c r="X4" s="99">
-        <f>Calculations!X4</f>
+        <f>Calculations!X4/SUM(Calculations!X$2:X$6)</f>
         <v>0</v>
       </c>
       <c r="Y4" s="99">
-        <f>Calculations!Y4</f>
+        <f>Calculations!Y4/SUM(Calculations!Y$2:Y$6)</f>
         <v>0</v>
       </c>
       <c r="Z4" s="99">
-        <f>Calculations!Z4</f>
+        <f>Calculations!Z4/SUM(Calculations!Z$2:Z$6)</f>
         <v>0</v>
       </c>
       <c r="AA4" s="99">
-        <f>Calculations!AA4</f>
+        <f>Calculations!AA4/SUM(Calculations!AA$2:AA$6)</f>
         <v>0</v>
       </c>
       <c r="AB4" s="99">
-        <f>Calculations!AB4</f>
+        <f>Calculations!AB4/SUM(Calculations!AB$2:AB$6)</f>
         <v>0</v>
       </c>
       <c r="AC4" s="99">
-        <f>Calculations!AC4</f>
+        <f>Calculations!AC4/SUM(Calculations!AC$2:AC$6)</f>
         <v>0</v>
       </c>
       <c r="AD4" s="99">
-        <f>Calculations!AD4</f>
+        <f>Calculations!AD4/SUM(Calculations!AD$2:AD$6)</f>
         <v>0</v>
       </c>
       <c r="AE4" s="99">
-        <f>Calculations!AE4</f>
+        <f>Calculations!AE4/SUM(Calculations!AE$2:AE$6)</f>
         <v>0</v>
       </c>
       <c r="AF4" s="99">
-        <f>Calculations!AF4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32">
+        <f>Calculations!AF4/SUM(Calculations!AF$2:AF$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>153</v>
       </c>
       <c r="B5" s="99">
-        <f>Calculations!B5</f>
+        <f>Calculations!B5/SUM(Calculations!B$2:B$6)</f>
         <v>0</v>
       </c>
       <c r="C5" s="99">
-        <f>Calculations!C5</f>
+        <f>Calculations!C5/SUM(Calculations!C$2:C$6)</f>
         <v>0</v>
       </c>
       <c r="D5" s="99">
-        <f>Calculations!D5</f>
+        <f>Calculations!D5/SUM(Calculations!D$2:D$6)</f>
         <v>0</v>
       </c>
       <c r="E5" s="99">
-        <f>Calculations!E5</f>
+        <f>Calculations!E5/SUM(Calculations!E$2:E$6)</f>
         <v>0</v>
       </c>
       <c r="F5" s="99">
-        <f>Calculations!F5</f>
+        <f>Calculations!F5/SUM(Calculations!F$2:F$6)</f>
         <v>0</v>
       </c>
       <c r="G5" s="99">
-        <f>Calculations!G5</f>
+        <f>Calculations!G5/SUM(Calculations!G$2:G$6)</f>
         <v>0</v>
       </c>
       <c r="H5" s="99">
-        <f>Calculations!H5</f>
+        <f>Calculations!H5/SUM(Calculations!H$2:H$6)</f>
         <v>0</v>
       </c>
       <c r="I5" s="99">
-        <f>Calculations!I5</f>
+        <f>Calculations!I5/SUM(Calculations!I$2:I$6)</f>
         <v>0</v>
       </c>
       <c r="J5" s="99">
-        <f>Calculations!J5</f>
+        <f>Calculations!J5/SUM(Calculations!J$2:J$6)</f>
         <v>0</v>
       </c>
       <c r="K5" s="99">
-        <f>Calculations!K5</f>
+        <f>Calculations!K5/SUM(Calculations!K$2:K$6)</f>
         <v>0</v>
       </c>
       <c r="L5" s="99">
-        <f>Calculations!L5</f>
+        <f>Calculations!L5/SUM(Calculations!L$2:L$6)</f>
         <v>0</v>
       </c>
       <c r="M5" s="99">
-        <f>Calculations!M5</f>
+        <f>Calculations!M5/SUM(Calculations!M$2:M$6)</f>
         <v>0</v>
       </c>
       <c r="N5" s="99">
-        <f>Calculations!N5</f>
+        <f>Calculations!N5/SUM(Calculations!N$2:N$6)</f>
         <v>0</v>
       </c>
       <c r="O5" s="99">
-        <f>Calculations!O5</f>
+        <f>Calculations!O5/SUM(Calculations!O$2:O$6)</f>
         <v>0</v>
       </c>
       <c r="P5" s="99">
-        <f>Calculations!P5</f>
+        <f>Calculations!P5/SUM(Calculations!P$2:P$6)</f>
         <v>0</v>
       </c>
       <c r="Q5" s="99">
-        <f>Calculations!Q5</f>
+        <f>Calculations!Q5/SUM(Calculations!Q$2:Q$6)</f>
         <v>0</v>
       </c>
       <c r="R5" s="99">
-        <f>Calculations!R5</f>
+        <f>Calculations!R5/SUM(Calculations!R$2:R$6)</f>
         <v>0</v>
       </c>
       <c r="S5" s="99">
-        <f>Calculations!S5</f>
+        <f>Calculations!S5/SUM(Calculations!S$2:S$6)</f>
         <v>0</v>
       </c>
       <c r="T5" s="99">
-        <f>Calculations!T5</f>
+        <f>Calculations!T5/SUM(Calculations!T$2:T$6)</f>
         <v>0</v>
       </c>
       <c r="U5" s="99">
-        <f>Calculations!U5</f>
+        <f>Calculations!U5/SUM(Calculations!U$2:U$6)</f>
         <v>0</v>
       </c>
       <c r="V5" s="99">
-        <f>Calculations!V5</f>
+        <f>Calculations!V5/SUM(Calculations!V$2:V$6)</f>
         <v>0</v>
       </c>
       <c r="W5" s="99">
-        <f>Calculations!W5</f>
+        <f>Calculations!W5/SUM(Calculations!W$2:W$6)</f>
         <v>0</v>
       </c>
       <c r="X5" s="99">
-        <f>Calculations!X5</f>
+        <f>Calculations!X5/SUM(Calculations!X$2:X$6)</f>
         <v>0</v>
       </c>
       <c r="Y5" s="99">
-        <f>Calculations!Y5</f>
+        <f>Calculations!Y5/SUM(Calculations!Y$2:Y$6)</f>
         <v>0</v>
       </c>
       <c r="Z5" s="99">
-        <f>Calculations!Z5</f>
+        <f>Calculations!Z5/SUM(Calculations!Z$2:Z$6)</f>
         <v>0</v>
       </c>
       <c r="AA5" s="99">
-        <f>Calculations!AA5</f>
+        <f>Calculations!AA5/SUM(Calculations!AA$2:AA$6)</f>
         <v>0</v>
       </c>
       <c r="AB5" s="99">
-        <f>Calculations!AB5</f>
+        <f>Calculations!AB5/SUM(Calculations!AB$2:AB$6)</f>
         <v>0</v>
       </c>
       <c r="AC5" s="99">
-        <f>Calculations!AC5</f>
+        <f>Calculations!AC5/SUM(Calculations!AC$2:AC$6)</f>
         <v>0</v>
       </c>
       <c r="AD5" s="99">
-        <f>Calculations!AD5</f>
+        <f>Calculations!AD5/SUM(Calculations!AD$2:AD$6)</f>
         <v>0</v>
       </c>
       <c r="AE5" s="99">
-        <f>Calculations!AE5</f>
+        <f>Calculations!AE5/SUM(Calculations!AE$2:AE$6)</f>
         <v>0</v>
       </c>
       <c r="AF5" s="99">
-        <f>Calculations!AF5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32">
+        <f>Calculations!AF5/SUM(Calculations!AF$2:AF$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>154</v>
       </c>
       <c r="B6" s="99">
-        <f>Calculations!B6</f>
+        <f>Calculations!B6/SUM(Calculations!B$2:B$6)</f>
         <v>0</v>
       </c>
       <c r="C6" s="99">
-        <f>Calculations!C6</f>
+        <f>Calculations!C6/SUM(Calculations!C$2:C$6)</f>
         <v>0</v>
       </c>
       <c r="D6" s="99">
-        <f>Calculations!D6</f>
+        <f>Calculations!D6/SUM(Calculations!D$2:D$6)</f>
         <v>0</v>
       </c>
       <c r="E6" s="99">
-        <f>Calculations!E6</f>
+        <f>Calculations!E6/SUM(Calculations!E$2:E$6)</f>
         <v>0</v>
       </c>
       <c r="F6" s="99">
-        <f>Calculations!F6</f>
+        <f>Calculations!F6/SUM(Calculations!F$2:F$6)</f>
         <v>0</v>
       </c>
       <c r="G6" s="99">
-        <f>Calculations!G6</f>
+        <f>Calculations!G6/SUM(Calculations!G$2:G$6)</f>
         <v>0</v>
       </c>
       <c r="H6" s="99">
-        <f>Calculations!H6</f>
+        <f>Calculations!H6/SUM(Calculations!H$2:H$6)</f>
         <v>0</v>
       </c>
       <c r="I6" s="99">
-        <f>Calculations!I6</f>
+        <f>Calculations!I6/SUM(Calculations!I$2:I$6)</f>
         <v>0</v>
       </c>
       <c r="J6" s="99">
-        <f>Calculations!J6</f>
+        <f>Calculations!J6/SUM(Calculations!J$2:J$6)</f>
         <v>0</v>
       </c>
       <c r="K6" s="99">
-        <f>Calculations!K6</f>
+        <f>Calculations!K6/SUM(Calculations!K$2:K$6)</f>
         <v>0</v>
       </c>
       <c r="L6" s="99">
-        <f>Calculations!L6</f>
+        <f>Calculations!L6/SUM(Calculations!L$2:L$6)</f>
         <v>0</v>
       </c>
       <c r="M6" s="99">
-        <f>Calculations!M6</f>
+        <f>Calculations!M6/SUM(Calculations!M$2:M$6)</f>
         <v>0</v>
       </c>
       <c r="N6" s="99">
-        <f>Calculations!N6</f>
+        <f>Calculations!N6/SUM(Calculations!N$2:N$6)</f>
         <v>0</v>
       </c>
       <c r="O6" s="99">
-        <f>Calculations!O6</f>
+        <f>Calculations!O6/SUM(Calculations!O$2:O$6)</f>
         <v>0</v>
       </c>
       <c r="P6" s="99">
-        <f>Calculations!P6</f>
+        <f>Calculations!P6/SUM(Calculations!P$2:P$6)</f>
         <v>0</v>
       </c>
       <c r="Q6" s="99">
-        <f>Calculations!Q6</f>
+        <f>Calculations!Q6/SUM(Calculations!Q$2:Q$6)</f>
         <v>0</v>
       </c>
       <c r="R6" s="99">
-        <f>Calculations!R6</f>
+        <f>Calculations!R6/SUM(Calculations!R$2:R$6)</f>
         <v>0</v>
       </c>
       <c r="S6" s="99">
-        <f>Calculations!S6</f>
+        <f>Calculations!S6/SUM(Calculations!S$2:S$6)</f>
         <v>0</v>
       </c>
       <c r="T6" s="99">
-        <f>Calculations!T6</f>
+        <f>Calculations!T6/SUM(Calculations!T$2:T$6)</f>
         <v>0</v>
       </c>
       <c r="U6" s="99">
-        <f>Calculations!U6</f>
+        <f>Calculations!U6/SUM(Calculations!U$2:U$6)</f>
         <v>0</v>
       </c>
       <c r="V6" s="99">
-        <f>Calculations!V6</f>
+        <f>Calculations!V6/SUM(Calculations!V$2:V$6)</f>
         <v>0</v>
       </c>
       <c r="W6" s="99">
-        <f>Calculations!W6</f>
+        <f>Calculations!W6/SUM(Calculations!W$2:W$6)</f>
         <v>0</v>
       </c>
       <c r="X6" s="99">
-        <f>Calculations!X6</f>
+        <f>Calculations!X6/SUM(Calculations!X$2:X$6)</f>
         <v>0</v>
       </c>
       <c r="Y6" s="99">
-        <f>Calculations!Y6</f>
+        <f>Calculations!Y6/SUM(Calculations!Y$2:Y$6)</f>
         <v>0</v>
       </c>
       <c r="Z6" s="99">
-        <f>Calculations!Z6</f>
+        <f>Calculations!Z6/SUM(Calculations!Z$2:Z$6)</f>
         <v>0</v>
       </c>
       <c r="AA6" s="99">
-        <f>Calculations!AA6</f>
+        <f>Calculations!AA6/SUM(Calculations!AA$2:AA$6)</f>
         <v>0</v>
       </c>
       <c r="AB6" s="99">
-        <f>Calculations!AB6</f>
+        <f>Calculations!AB6/SUM(Calculations!AB$2:AB$6)</f>
         <v>0</v>
       </c>
       <c r="AC6" s="99">
-        <f>Calculations!AC6</f>
+        <f>Calculations!AC6/SUM(Calculations!AC$2:AC$6)</f>
         <v>0</v>
       </c>
       <c r="AD6" s="99">
-        <f>Calculations!AD6</f>
+        <f>Calculations!AD6/SUM(Calculations!AD$2:AD$6)</f>
         <v>0</v>
       </c>
       <c r="AE6" s="99">
-        <f>Calculations!AE6</f>
+        <f>Calculations!AE6/SUM(Calculations!AE$2:AE$6)</f>
         <v>0</v>
       </c>
       <c r="AF6" s="99">
-        <f>Calculations!AF6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" ht="15">
+        <f>Calculations!AF6/SUM(Calculations!AF$2:AF$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -12662,7 +12680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" ht="15">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>161</v>
       </c>
@@ -12760,34 +12778,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="15"/>
-    <row r="16" spans="1:32" ht="15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -13016,14 +13012,60 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEA4C8E-9D8C-453A-8E5F-02C5C3A31D99}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC96DCF2-3D6F-413B-88E1-2B27BC1128F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D3E8F0-5A13-4AED-8799-E0B85C663863}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D3E8F0-5A13-4AED-8799-E0B85C663863}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC96DCF2-3D6F-413B-88E1-2B27BC1128F2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEA4C8E-9D8C-453A-8E5F-02C5C3A31D99}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixes reference error in SMR vs POx shares
</commit_message>
<xml_diff>
--- a/InputData/hydgn/BHPSbP/BAU Hydrogen Production Shr by Pathway.xlsx
+++ b/InputData/hydgn/BHPSbP/BAU Hydrogen Production Shr by Pathway.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\hydgn\BHPSbP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CF4CE2-64CA-4A07-95EF-AD8C17B102BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78824979-273D-4058-8BE3-8BBEA84B18F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30930" yWindow="3390" windowWidth="23025" windowHeight="13470" tabRatio="685" firstSheet="2" activeTab="7" xr2:uid="{507E633D-E752-41BB-B866-72E946289DF3}"/>
+    <workbookView xWindow="60930" yWindow="1635" windowWidth="23025" windowHeight="13440" tabRatio="685" firstSheet="2" activeTab="7" xr2:uid="{507E633D-E752-41BB-B866-72E946289DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -3892,30 +3892,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="21" fillId="8" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="8" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3934,6 +3910,30 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="24" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="21" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="8" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="8" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -6991,11 +6991,6 @@
             <v>3412000000</v>
           </cell>
         </row>
-        <row r="188">
-          <cell r="C188">
-            <v>134509803921568.64</v>
-          </cell>
-        </row>
       </sheetData>
       <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2" refreshError="1"/>
@@ -17382,238 +17377,238 @@
       </c>
     </row>
     <row r="122" spans="1:14" s="34" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A122" s="268" t="s">
+      <c r="A122" s="278" t="s">
         <v>105</v>
       </c>
-      <c r="B122" s="269"/>
-      <c r="C122" s="269"/>
-      <c r="D122" s="269"/>
-      <c r="E122" s="269"/>
-      <c r="F122" s="269"/>
-      <c r="G122" s="269"/>
-      <c r="H122" s="269"/>
-      <c r="I122" s="269"/>
-      <c r="J122" s="269"/>
-      <c r="K122" s="269"/>
-      <c r="L122" s="269"/>
-      <c r="M122" s="269"/>
-      <c r="N122" s="269"/>
+      <c r="B122" s="279"/>
+      <c r="C122" s="279"/>
+      <c r="D122" s="279"/>
+      <c r="E122" s="279"/>
+      <c r="F122" s="279"/>
+      <c r="G122" s="279"/>
+      <c r="H122" s="279"/>
+      <c r="I122" s="279"/>
+      <c r="J122" s="279"/>
+      <c r="K122" s="279"/>
+      <c r="L122" s="279"/>
+      <c r="M122" s="279"/>
+      <c r="N122" s="279"/>
     </row>
     <row r="123" spans="1:14" s="34" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="266" t="s">
+      <c r="A123" s="276" t="s">
         <v>106</v>
       </c>
-      <c r="B123" s="266"/>
-      <c r="C123" s="266"/>
-      <c r="D123" s="266"/>
-      <c r="E123" s="266"/>
-      <c r="F123" s="266"/>
-      <c r="G123" s="266"/>
-      <c r="H123" s="266"/>
-      <c r="I123" s="266"/>
-      <c r="J123" s="266"/>
-      <c r="K123" s="266"/>
-      <c r="L123" s="266"/>
-      <c r="M123" s="266"/>
-      <c r="N123" s="266"/>
+      <c r="B123" s="276"/>
+      <c r="C123" s="276"/>
+      <c r="D123" s="276"/>
+      <c r="E123" s="276"/>
+      <c r="F123" s="276"/>
+      <c r="G123" s="276"/>
+      <c r="H123" s="276"/>
+      <c r="I123" s="276"/>
+      <c r="J123" s="276"/>
+      <c r="K123" s="276"/>
+      <c r="L123" s="276"/>
+      <c r="M123" s="276"/>
+      <c r="N123" s="276"/>
     </row>
     <row r="124" spans="1:14" s="34" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A124" s="266" t="s">
+      <c r="A124" s="276" t="s">
         <v>107</v>
       </c>
-      <c r="B124" s="267"/>
-      <c r="C124" s="267"/>
-      <c r="D124" s="267"/>
-      <c r="E124" s="267"/>
-      <c r="F124" s="267"/>
-      <c r="G124" s="267"/>
-      <c r="H124" s="267"/>
-      <c r="I124" s="267"/>
-      <c r="J124" s="267"/>
-      <c r="K124" s="267"/>
-      <c r="L124" s="267"/>
-      <c r="M124" s="267"/>
-      <c r="N124" s="267"/>
+      <c r="B124" s="277"/>
+      <c r="C124" s="277"/>
+      <c r="D124" s="277"/>
+      <c r="E124" s="277"/>
+      <c r="F124" s="277"/>
+      <c r="G124" s="277"/>
+      <c r="H124" s="277"/>
+      <c r="I124" s="277"/>
+      <c r="J124" s="277"/>
+      <c r="K124" s="277"/>
+      <c r="L124" s="277"/>
+      <c r="M124" s="277"/>
+      <c r="N124" s="277"/>
     </row>
     <row r="125" spans="1:14" s="34" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A125" s="266" t="s">
+      <c r="A125" s="276" t="s">
         <v>108</v>
       </c>
-      <c r="B125" s="267"/>
-      <c r="C125" s="267"/>
-      <c r="D125" s="267"/>
-      <c r="E125" s="267"/>
-      <c r="F125" s="267"/>
-      <c r="G125" s="267"/>
-      <c r="H125" s="267"/>
-      <c r="I125" s="267"/>
-      <c r="J125" s="267"/>
-      <c r="K125" s="267"/>
-      <c r="L125" s="267"/>
-      <c r="M125" s="267"/>
-      <c r="N125" s="267"/>
+      <c r="B125" s="277"/>
+      <c r="C125" s="277"/>
+      <c r="D125" s="277"/>
+      <c r="E125" s="277"/>
+      <c r="F125" s="277"/>
+      <c r="G125" s="277"/>
+      <c r="H125" s="277"/>
+      <c r="I125" s="277"/>
+      <c r="J125" s="277"/>
+      <c r="K125" s="277"/>
+      <c r="L125" s="277"/>
+      <c r="M125" s="277"/>
+      <c r="N125" s="277"/>
     </row>
     <row r="126" spans="1:14" s="34" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A126" s="266" t="s">
+      <c r="A126" s="276" t="s">
         <v>109</v>
       </c>
-      <c r="B126" s="267"/>
-      <c r="C126" s="267"/>
-      <c r="D126" s="267"/>
-      <c r="E126" s="267"/>
-      <c r="F126" s="267"/>
-      <c r="G126" s="267"/>
-      <c r="H126" s="267"/>
-      <c r="I126" s="267"/>
-      <c r="J126" s="267"/>
-      <c r="K126" s="267"/>
-      <c r="L126" s="267"/>
-      <c r="M126" s="267"/>
-      <c r="N126" s="267"/>
+      <c r="B126" s="277"/>
+      <c r="C126" s="277"/>
+      <c r="D126" s="277"/>
+      <c r="E126" s="277"/>
+      <c r="F126" s="277"/>
+      <c r="G126" s="277"/>
+      <c r="H126" s="277"/>
+      <c r="I126" s="277"/>
+      <c r="J126" s="277"/>
+      <c r="K126" s="277"/>
+      <c r="L126" s="277"/>
+      <c r="M126" s="277"/>
+      <c r="N126" s="277"/>
     </row>
     <row r="127" spans="1:14" s="34" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A127" s="266" t="s">
+      <c r="A127" s="276" t="s">
         <v>110</v>
       </c>
-      <c r="B127" s="267"/>
-      <c r="C127" s="267"/>
-      <c r="D127" s="267"/>
-      <c r="E127" s="267"/>
-      <c r="F127" s="267"/>
-      <c r="G127" s="267"/>
-      <c r="H127" s="267"/>
-      <c r="I127" s="267"/>
-      <c r="J127" s="267"/>
-      <c r="K127" s="267"/>
-      <c r="L127" s="267"/>
-      <c r="M127" s="267"/>
-      <c r="N127" s="267"/>
+      <c r="B127" s="277"/>
+      <c r="C127" s="277"/>
+      <c r="D127" s="277"/>
+      <c r="E127" s="277"/>
+      <c r="F127" s="277"/>
+      <c r="G127" s="277"/>
+      <c r="H127" s="277"/>
+      <c r="I127" s="277"/>
+      <c r="J127" s="277"/>
+      <c r="K127" s="277"/>
+      <c r="L127" s="277"/>
+      <c r="M127" s="277"/>
+      <c r="N127" s="277"/>
     </row>
     <row r="128" spans="1:14" s="34" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A128" s="266" t="s">
+      <c r="A128" s="276" t="s">
         <v>111</v>
       </c>
-      <c r="B128" s="267"/>
-      <c r="C128" s="267"/>
-      <c r="D128" s="267"/>
-      <c r="E128" s="267"/>
-      <c r="F128" s="267"/>
-      <c r="G128" s="267"/>
-      <c r="H128" s="267"/>
-      <c r="I128" s="267"/>
-      <c r="J128" s="267"/>
-      <c r="K128" s="267"/>
-      <c r="L128" s="267"/>
-      <c r="M128" s="267"/>
-      <c r="N128" s="267"/>
+      <c r="B128" s="277"/>
+      <c r="C128" s="277"/>
+      <c r="D128" s="277"/>
+      <c r="E128" s="277"/>
+      <c r="F128" s="277"/>
+      <c r="G128" s="277"/>
+      <c r="H128" s="277"/>
+      <c r="I128" s="277"/>
+      <c r="J128" s="277"/>
+      <c r="K128" s="277"/>
+      <c r="L128" s="277"/>
+      <c r="M128" s="277"/>
+      <c r="N128" s="277"/>
     </row>
     <row r="129" spans="1:14" s="34" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A129" s="266" t="s">
+      <c r="A129" s="276" t="s">
         <v>112</v>
       </c>
-      <c r="B129" s="267"/>
-      <c r="C129" s="267"/>
-      <c r="D129" s="267"/>
-      <c r="E129" s="267"/>
-      <c r="F129" s="267"/>
-      <c r="G129" s="267"/>
-      <c r="H129" s="267"/>
-      <c r="I129" s="267"/>
-      <c r="J129" s="267"/>
-      <c r="K129" s="267"/>
-      <c r="L129" s="267"/>
-      <c r="M129" s="267"/>
-      <c r="N129" s="267"/>
+      <c r="B129" s="277"/>
+      <c r="C129" s="277"/>
+      <c r="D129" s="277"/>
+      <c r="E129" s="277"/>
+      <c r="F129" s="277"/>
+      <c r="G129" s="277"/>
+      <c r="H129" s="277"/>
+      <c r="I129" s="277"/>
+      <c r="J129" s="277"/>
+      <c r="K129" s="277"/>
+      <c r="L129" s="277"/>
+      <c r="M129" s="277"/>
+      <c r="N129" s="277"/>
     </row>
     <row r="130" spans="1:14" s="34" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A130" s="266" t="s">
+      <c r="A130" s="276" t="s">
         <v>113</v>
       </c>
-      <c r="B130" s="267"/>
-      <c r="C130" s="267"/>
-      <c r="D130" s="267"/>
-      <c r="E130" s="267"/>
-      <c r="F130" s="267"/>
-      <c r="G130" s="267"/>
-      <c r="H130" s="267"/>
-      <c r="I130" s="267"/>
-      <c r="J130" s="267"/>
-      <c r="K130" s="267"/>
-      <c r="L130" s="267"/>
-      <c r="M130" s="267"/>
-      <c r="N130" s="267"/>
+      <c r="B130" s="277"/>
+      <c r="C130" s="277"/>
+      <c r="D130" s="277"/>
+      <c r="E130" s="277"/>
+      <c r="F130" s="277"/>
+      <c r="G130" s="277"/>
+      <c r="H130" s="277"/>
+      <c r="I130" s="277"/>
+      <c r="J130" s="277"/>
+      <c r="K130" s="277"/>
+      <c r="L130" s="277"/>
+      <c r="M130" s="277"/>
+      <c r="N130" s="277"/>
     </row>
     <row r="131" spans="1:14" s="34" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A131" s="266" t="s">
+      <c r="A131" s="276" t="s">
         <v>114</v>
       </c>
-      <c r="B131" s="267"/>
-      <c r="C131" s="267"/>
-      <c r="D131" s="267"/>
-      <c r="E131" s="267"/>
-      <c r="F131" s="267"/>
-      <c r="G131" s="267"/>
-      <c r="H131" s="267"/>
-      <c r="I131" s="267"/>
-      <c r="J131" s="267"/>
-      <c r="K131" s="267"/>
-      <c r="L131" s="267"/>
-      <c r="M131" s="267"/>
-      <c r="N131" s="267"/>
+      <c r="B131" s="277"/>
+      <c r="C131" s="277"/>
+      <c r="D131" s="277"/>
+      <c r="E131" s="277"/>
+      <c r="F131" s="277"/>
+      <c r="G131" s="277"/>
+      <c r="H131" s="277"/>
+      <c r="I131" s="277"/>
+      <c r="J131" s="277"/>
+      <c r="K131" s="277"/>
+      <c r="L131" s="277"/>
+      <c r="M131" s="277"/>
+      <c r="N131" s="277"/>
     </row>
     <row r="132" spans="1:14" s="34" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A132" s="266" t="s">
+      <c r="A132" s="276" t="s">
         <v>115</v>
       </c>
-      <c r="B132" s="267"/>
-      <c r="C132" s="267"/>
-      <c r="D132" s="267"/>
-      <c r="E132" s="267"/>
-      <c r="F132" s="267"/>
-      <c r="G132" s="267"/>
-      <c r="H132" s="267"/>
-      <c r="I132" s="267"/>
-      <c r="J132" s="267"/>
-      <c r="K132" s="267"/>
-      <c r="L132" s="267"/>
-      <c r="M132" s="267"/>
-      <c r="N132" s="267"/>
+      <c r="B132" s="277"/>
+      <c r="C132" s="277"/>
+      <c r="D132" s="277"/>
+      <c r="E132" s="277"/>
+      <c r="F132" s="277"/>
+      <c r="G132" s="277"/>
+      <c r="H132" s="277"/>
+      <c r="I132" s="277"/>
+      <c r="J132" s="277"/>
+      <c r="K132" s="277"/>
+      <c r="L132" s="277"/>
+      <c r="M132" s="277"/>
+      <c r="N132" s="277"/>
     </row>
     <row r="133" spans="1:14" s="34" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A133" s="266" t="s">
+      <c r="A133" s="276" t="s">
         <v>116</v>
       </c>
-      <c r="B133" s="267"/>
-      <c r="C133" s="267"/>
-      <c r="D133" s="267"/>
-      <c r="E133" s="267"/>
-      <c r="F133" s="267"/>
-      <c r="G133" s="267"/>
-      <c r="H133" s="267"/>
-      <c r="I133" s="267"/>
-      <c r="J133" s="267"/>
-      <c r="K133" s="267"/>
-      <c r="L133" s="267"/>
-      <c r="M133" s="267"/>
-      <c r="N133" s="267"/>
+      <c r="B133" s="277"/>
+      <c r="C133" s="277"/>
+      <c r="D133" s="277"/>
+      <c r="E133" s="277"/>
+      <c r="F133" s="277"/>
+      <c r="G133" s="277"/>
+      <c r="H133" s="277"/>
+      <c r="I133" s="277"/>
+      <c r="J133" s="277"/>
+      <c r="K133" s="277"/>
+      <c r="L133" s="277"/>
+      <c r="M133" s="277"/>
+      <c r="N133" s="277"/>
     </row>
     <row r="134" spans="1:14" s="34" customFormat="1" ht="9.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="264" t="s">
+      <c r="A134" s="280" t="s">
         <v>117</v>
       </c>
-      <c r="B134" s="265"/>
-      <c r="C134" s="265"/>
-      <c r="D134" s="265"/>
-      <c r="E134" s="265"/>
-      <c r="F134" s="265"/>
-      <c r="G134" s="265"/>
-      <c r="H134" s="265"/>
-      <c r="I134" s="265"/>
-      <c r="J134" s="265"/>
-      <c r="K134" s="265"/>
-      <c r="L134" s="265"/>
-      <c r="M134" s="265"/>
-      <c r="N134" s="265"/>
+      <c r="B134" s="281"/>
+      <c r="C134" s="281"/>
+      <c r="D134" s="281"/>
+      <c r="E134" s="281"/>
+      <c r="F134" s="281"/>
+      <c r="G134" s="281"/>
+      <c r="H134" s="281"/>
+      <c r="I134" s="281"/>
+      <c r="J134" s="281"/>
+      <c r="K134" s="281"/>
+      <c r="L134" s="281"/>
+      <c r="M134" s="281"/>
+      <c r="N134" s="281"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="35" t="s">
@@ -17632,12 +17627,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A127:N127"/>
-    <mergeCell ref="A122:N122"/>
-    <mergeCell ref="A123:N123"/>
-    <mergeCell ref="A124:N124"/>
-    <mergeCell ref="A125:N125"/>
-    <mergeCell ref="A126:N126"/>
     <mergeCell ref="A134:N134"/>
     <mergeCell ref="A128:N128"/>
     <mergeCell ref="A129:N129"/>
@@ -17645,6 +17634,12 @@
     <mergeCell ref="A131:N131"/>
     <mergeCell ref="A132:N132"/>
     <mergeCell ref="A133:N133"/>
+    <mergeCell ref="A127:N127"/>
+    <mergeCell ref="A122:N122"/>
+    <mergeCell ref="A123:N123"/>
+    <mergeCell ref="A124:N124"/>
+    <mergeCell ref="A125:N125"/>
+    <mergeCell ref="A126:N126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17715,7 +17710,7 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17727,39 +17722,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="283" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
+      <c r="B1" s="283"/>
+      <c r="C1" s="283"/>
+      <c r="D1" s="283"/>
+      <c r="E1" s="283"/>
+      <c r="F1" s="283"/>
+      <c r="G1" s="283"/>
+      <c r="H1" s="283"/>
+      <c r="I1" s="283"/>
+      <c r="J1" s="283"/>
+      <c r="K1" s="283"/>
+      <c r="L1" s="283"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="270" t="s">
+      <c r="C3" s="282" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="270"/>
-      <c r="E3" s="270"/>
-      <c r="F3" s="270" t="s">
+      <c r="D3" s="282"/>
+      <c r="E3" s="282"/>
+      <c r="F3" s="282" t="s">
         <v>126</v>
       </c>
-      <c r="G3" s="270"/>
-      <c r="H3" s="270"/>
-      <c r="I3" s="270" t="s">
+      <c r="G3" s="282"/>
+      <c r="H3" s="282"/>
+      <c r="I3" s="282" t="s">
         <v>127</v>
       </c>
-      <c r="J3" s="270"/>
-      <c r="K3" s="270"/>
+      <c r="J3" s="282"/>
+      <c r="K3" s="282"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="9"/>
@@ -18308,7 +18303,7 @@
   <dimension ref="A1:AH76"/>
   <sheetViews>
     <sheetView topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18360,7 +18355,7 @@
       </c>
       <c r="E2" s="259"/>
     </row>
-    <row r="3" spans="1:8" s="272" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="264" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="260" t="s">
         <v>363</v>
       </c>
@@ -18380,7 +18375,6 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <f>C4*[1]About!C$188</f>
         <v>403529411764705.94</v>
       </c>
       <c r="E4" s="259" t="s">
@@ -18398,7 +18392,6 @@
         <v>0.5</v>
       </c>
       <c r="D5">
-        <f>C5*[1]About!C$188</f>
         <v>67254901960784.32</v>
       </c>
       <c r="E5" s="259" t="s">
@@ -18416,7 +18409,6 @@
         <v>0.6</v>
       </c>
       <c r="D6">
-        <f>C6*[1]About!C$188</f>
         <v>80705882352941.188</v>
       </c>
       <c r="E6" s="259" t="s">
@@ -18434,7 +18426,6 @@
         <v>1.4</v>
       </c>
       <c r="D7">
-        <f>C7*[1]About!C$188</f>
         <v>188313725490196.09</v>
       </c>
       <c r="E7" s="259" t="s">
@@ -18446,37 +18437,37 @@
         <f>SUM(C4:C7)</f>
         <v>5.5</v>
       </c>
-      <c r="H8" s="273"/>
+      <c r="H8" s="265"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="97" t="s">
         <v>373</v>
       </c>
-      <c r="H9" s="274"/>
+      <c r="H9" s="266"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="97" t="s">
         <v>371</v>
       </c>
-      <c r="H10" s="274"/>
+      <c r="H10" s="266"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H11" s="274"/>
+      <c r="H11" s="266"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H12" s="274"/>
+      <c r="H12" s="266"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C13" s="200"/>
-      <c r="H13" s="274"/>
+      <c r="H13" s="266"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C14" s="200"/>
-      <c r="H14" s="274"/>
+      <c r="H14" s="266"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C15" s="200"/>
-      <c r="H15" s="274"/>
+      <c r="H15" s="266"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="82"/>
@@ -18490,26 +18481,26 @@
       </c>
     </row>
     <row r="35" spans="1:34" s="261" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="275" t="s">
+      <c r="A35" s="267" t="s">
         <v>359</v>
       </c>
-      <c r="B35" s="275" t="s">
+      <c r="B35" s="267" t="s">
         <v>360</v>
       </c>
-      <c r="C35" s="276" t="s">
+      <c r="C35" s="268" t="s">
         <v>375</v>
       </c>
-      <c r="D35" s="276" t="s">
+      <c r="D35" s="268" t="s">
         <v>376</v>
       </c>
-      <c r="E35" s="276" t="s">
+      <c r="E35" s="268" t="s">
         <v>377</v>
       </c>
-      <c r="F35" s="276" t="s">
+      <c r="F35" s="268" t="s">
         <v>378</v>
       </c>
-      <c r="G35" s="276"/>
-      <c r="H35" s="276"/>
+      <c r="G35" s="268"/>
+      <c r="H35" s="268"/>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
@@ -18608,7 +18599,7 @@
       <c r="C41" s="97"/>
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A42" s="277" t="s">
+      <c r="A42" s="269" t="s">
         <v>380</v>
       </c>
       <c r="C42" s="97">
@@ -19132,7 +19123,7 @@
         <v>chemicals 20</v>
       </c>
       <c r="C46" s="97">
-        <f t="shared" ref="C46" si="2">D39</f>
+        <f>D39</f>
         <v>188313725490196.09</v>
       </c>
       <c r="D46">
@@ -19268,9 +19259,13 @@
     </row>
     <row r="48" spans="1:34" x14ac:dyDescent="0.35">
       <c r="C48" s="97"/>
+      <c r="F48">
+        <f>SUM(F43:F44,F46)</f>
+        <v>672241147106237.75</v>
+      </c>
     </row>
     <row r="49" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A49" s="277" t="s">
+      <c r="A49" s="269" t="s">
         <v>382</v>
       </c>
       <c r="C49" s="97"/>
@@ -19378,131 +19373,131 @@
         <v>366</v>
       </c>
       <c r="C51">
-        <f t="shared" ref="C51:R52" si="3">SUMIFS(C$43:C$46,$B$43:$B$46,$B51)</f>
+        <f t="shared" ref="C51:R52" si="2">SUMIFS(C$43:C$46,$B$43:$B$46,$B51)</f>
         <v>147960784313725.5</v>
       </c>
       <c r="D51">
+        <f t="shared" si="2"/>
+        <v>147123248419922.56</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>146826240904252.5</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="2"/>
+        <v>145975164551731.94</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="2"/>
+        <v>144896979049919</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="2"/>
+        <v>143535323436791.53</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="2"/>
+        <v>142359288368324.09</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="2"/>
+        <v>141640945295947.47</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="2"/>
+        <v>140577690808586.81</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="2"/>
+        <v>140074339761915.84</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="2"/>
+        <v>139470128126182.38</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="2"/>
+        <v>138559242042264.22</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="2"/>
+        <v>138175890171801.72</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="2"/>
+        <v>137597734025555.25</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="2"/>
+        <v>136813922620747.41</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="2"/>
+        <v>136033117210035.63</v>
+      </c>
+      <c r="S51">
+        <f t="shared" ref="S51:AH52" si="3">SUMIFS(S$43:S$46,$B$43:$B$46,$B51)</f>
+        <v>134635579487534.56</v>
+      </c>
+      <c r="T51">
         <f t="shared" si="3"/>
-        <v>147123248419922.56</v>
-      </c>
-      <c r="E51">
+        <v>134192586903683.88</v>
+      </c>
+      <c r="U51">
         <f t="shared" si="3"/>
-        <v>146826240904252.5</v>
-      </c>
-      <c r="F51">
+        <v>133050505620655.41</v>
+      </c>
+      <c r="V51">
         <f t="shared" si="3"/>
-        <v>145975164551731.94</v>
-      </c>
-      <c r="G51">
+        <v>132110743868592.03</v>
+      </c>
+      <c r="W51">
         <f t="shared" si="3"/>
-        <v>144896979049919</v>
-      </c>
-      <c r="H51">
+        <v>131110782758958.69</v>
+      </c>
+      <c r="X51">
         <f t="shared" si="3"/>
-        <v>143535323436791.53</v>
-      </c>
-      <c r="I51">
+        <v>130058798990318.25</v>
+      </c>
+      <c r="Y51">
         <f t="shared" si="3"/>
-        <v>142359288368324.09</v>
-      </c>
-      <c r="J51">
+        <v>128673879247553.06</v>
+      </c>
+      <c r="Z51">
         <f t="shared" si="3"/>
-        <v>141640945295947.47</v>
-      </c>
-      <c r="K51">
+        <v>127658310422180.78</v>
+      </c>
+      <c r="AA51">
         <f t="shared" si="3"/>
-        <v>140577690808586.81</v>
-      </c>
-      <c r="L51">
+        <v>126339471149552.66</v>
+      </c>
+      <c r="AB51">
         <f t="shared" si="3"/>
-        <v>140074339761915.84</v>
-      </c>
-      <c r="M51">
+        <v>125241087203681.84</v>
+      </c>
+      <c r="AC51">
         <f t="shared" si="3"/>
-        <v>139470128126182.38</v>
-      </c>
-      <c r="N51">
+        <v>124326294834192.19</v>
+      </c>
+      <c r="AD51">
         <f t="shared" si="3"/>
-        <v>138559242042264.22</v>
-      </c>
-      <c r="O51">
+        <v>123480441151643.03</v>
+      </c>
+      <c r="AE51">
         <f t="shared" si="3"/>
-        <v>138175890171801.72</v>
-      </c>
-      <c r="P51">
+        <v>122305159709826.13</v>
+      </c>
+      <c r="AF51">
         <f t="shared" si="3"/>
-        <v>137597734025555.25</v>
-      </c>
-      <c r="Q51">
+        <v>121400271553696.22</v>
+      </c>
+      <c r="AG51">
         <f t="shared" si="3"/>
-        <v>136813922620747.41</v>
-      </c>
-      <c r="R51">
+        <v>120475489968803.28</v>
+      </c>
+      <c r="AH51">
         <f t="shared" si="3"/>
-        <v>136033117210035.63</v>
-      </c>
-      <c r="S51">
-        <f t="shared" ref="S51:AH52" si="4">SUMIFS(S$43:S$46,$B$43:$B$46,$B51)</f>
-        <v>134635579487534.56</v>
-      </c>
-      <c r="T51">
-        <f t="shared" si="4"/>
-        <v>134192586903683.88</v>
-      </c>
-      <c r="U51">
-        <f t="shared" si="4"/>
-        <v>133050505620655.41</v>
-      </c>
-      <c r="V51">
-        <f t="shared" si="4"/>
-        <v>132110743868592.03</v>
-      </c>
-      <c r="W51">
-        <f t="shared" si="4"/>
-        <v>131110782758958.69</v>
-      </c>
-      <c r="X51">
-        <f t="shared" si="4"/>
-        <v>130058798990318.25</v>
-      </c>
-      <c r="Y51">
-        <f t="shared" si="4"/>
-        <v>128673879247553.06</v>
-      </c>
-      <c r="Z51">
-        <f t="shared" si="4"/>
-        <v>127658310422180.78</v>
-      </c>
-      <c r="AA51">
-        <f t="shared" si="4"/>
-        <v>126339471149552.66</v>
-      </c>
-      <c r="AB51">
-        <f t="shared" si="4"/>
-        <v>125241087203681.84</v>
-      </c>
-      <c r="AC51">
-        <f t="shared" si="4"/>
-        <v>124326294834192.19</v>
-      </c>
-      <c r="AD51">
-        <f t="shared" si="4"/>
-        <v>123480441151643.03</v>
-      </c>
-      <c r="AE51">
-        <f t="shared" si="4"/>
-        <v>122305159709826.13</v>
-      </c>
-      <c r="AF51">
-        <f t="shared" si="4"/>
-        <v>121400271553696.22</v>
-      </c>
-      <c r="AG51">
-        <f t="shared" si="4"/>
-        <v>120475489968803.28</v>
-      </c>
-      <c r="AH51">
-        <f t="shared" si="4"/>
         <v>119291217423400.66</v>
       </c>
     </row>
@@ -19511,131 +19506,131 @@
         <v>365</v>
       </c>
       <c r="C52">
+        <f>SUMIFS(C$43:C$46,$B$43:$B$46,$B52)</f>
+        <v>591843137254902</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="2"/>
+        <v>597385051645088.38</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>601768431154983.5</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="2"/>
+        <v>605888799582723.25</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="2"/>
+        <v>608527563831442.5</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="2"/>
+        <v>609671551015228</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="2"/>
+        <v>611549452528532.38</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="2"/>
+        <v>614140822690759.25</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="2"/>
+        <v>616289753051685</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="2"/>
+        <v>618748480162494.25</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="2"/>
+        <v>620671456494360.75</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="2"/>
+        <v>621596890194579.25</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="2"/>
+        <v>623829896619109.63</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="2"/>
+        <v>625341414760584.13</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="2"/>
+        <v>626644896948488.88</v>
+      </c>
+      <c r="R52">
+        <f t="shared" si="2"/>
+        <v>627593386399401</v>
+      </c>
+      <c r="S52">
         <f t="shared" si="3"/>
-        <v>591843137254902</v>
-      </c>
-      <c r="D52">
+        <v>627520240881074.75</v>
+      </c>
+      <c r="T52">
         <f t="shared" si="3"/>
-        <v>597385051645088.38</v>
-      </c>
-      <c r="E52">
+        <v>629352457101693.88</v>
+      </c>
+      <c r="U52">
         <f t="shared" si="3"/>
-        <v>601768431154983.5</v>
-      </c>
-      <c r="F52">
+        <v>630182392418278.13</v>
+      </c>
+      <c r="V52">
         <f t="shared" si="3"/>
-        <v>605888799582723.25</v>
-      </c>
-      <c r="G52">
+        <v>631464957797512</v>
+      </c>
+      <c r="W52">
         <f t="shared" si="3"/>
-        <v>608527563831442.5</v>
-      </c>
-      <c r="H52">
+        <v>632482274073076.5</v>
+      </c>
+      <c r="X52">
         <f t="shared" si="3"/>
-        <v>609671551015228</v>
-      </c>
-      <c r="I52">
+        <v>633683507824757</v>
+      </c>
+      <c r="Y52">
         <f t="shared" si="3"/>
-        <v>611549452528532.38</v>
-      </c>
-      <c r="J52">
+        <v>634499239699560.38</v>
+      </c>
+      <c r="Z52">
         <f t="shared" si="3"/>
-        <v>614140822690759.25</v>
-      </c>
-      <c r="K52">
+        <v>636326655784091.25</v>
+      </c>
+      <c r="AA52">
         <f t="shared" si="3"/>
-        <v>616289753051685</v>
-      </c>
-      <c r="L52">
+        <v>637163588254378.25</v>
+      </c>
+      <c r="AB52">
         <f t="shared" si="3"/>
-        <v>618748480162494.25</v>
-      </c>
-      <c r="M52">
+        <v>638648875705799.88</v>
+      </c>
+      <c r="AC52">
         <f t="shared" si="3"/>
-        <v>620671456494360.75</v>
-      </c>
-      <c r="N52">
+        <v>639524240926516</v>
+      </c>
+      <c r="AD52">
         <f t="shared" si="3"/>
-        <v>621596890194579.25</v>
-      </c>
-      <c r="O52">
+        <v>641302989333804</v>
+      </c>
+      <c r="AE52">
         <f t="shared" si="3"/>
-        <v>623829896619109.63</v>
-      </c>
-      <c r="P52">
+        <v>642497203433983</v>
+      </c>
+      <c r="AF52">
         <f t="shared" si="3"/>
-        <v>625341414760584.13</v>
-      </c>
-      <c r="Q52">
+        <v>644030571307524</v>
+      </c>
+      <c r="AG52">
         <f t="shared" si="3"/>
-        <v>626644896948488.88</v>
-      </c>
-      <c r="R52">
+        <v>645210922957752.13</v>
+      </c>
+      <c r="AH52">
         <f t="shared" si="3"/>
-        <v>627593386399401</v>
-      </c>
-      <c r="S52">
-        <f t="shared" si="4"/>
-        <v>627520240881074.75</v>
-      </c>
-      <c r="T52">
-        <f t="shared" si="4"/>
-        <v>629352457101693.88</v>
-      </c>
-      <c r="U52">
-        <f t="shared" si="4"/>
-        <v>630182392418278.13</v>
-      </c>
-      <c r="V52">
-        <f t="shared" si="4"/>
-        <v>631464957797512</v>
-      </c>
-      <c r="W52">
-        <f t="shared" si="4"/>
-        <v>632482274073076.5</v>
-      </c>
-      <c r="X52">
-        <f t="shared" si="4"/>
-        <v>633683507824757</v>
-      </c>
-      <c r="Y52">
-        <f t="shared" si="4"/>
-        <v>634499239699560.38</v>
-      </c>
-      <c r="Z52">
-        <f t="shared" si="4"/>
-        <v>636326655784091.25</v>
-      </c>
-      <c r="AA52">
-        <f t="shared" si="4"/>
-        <v>637163588254378.25</v>
-      </c>
-      <c r="AB52">
-        <f t="shared" si="4"/>
-        <v>638648875705799.88</v>
-      </c>
-      <c r="AC52">
-        <f t="shared" si="4"/>
-        <v>639524240926516</v>
-      </c>
-      <c r="AD52">
-        <f t="shared" si="4"/>
-        <v>641302989333804</v>
-      </c>
-      <c r="AE52">
-        <f t="shared" si="4"/>
-        <v>642497203433983</v>
-      </c>
-      <c r="AF52">
-        <f t="shared" si="4"/>
-        <v>644030571307524</v>
-      </c>
-      <c r="AG52">
-        <f t="shared" si="4"/>
-        <v>645210922957752.13</v>
-      </c>
-      <c r="AH52">
-        <f t="shared" si="4"/>
         <v>646008127695636.63</v>
       </c>
     </row>
@@ -19741,97 +19736,97 @@
       <c r="A55" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B55" s="278">
+      <c r="B55" s="270">
         <v>5.3213834166182343E-5</v>
       </c>
-      <c r="C55" s="278">
+      <c r="C55" s="270">
         <v>6.8793532593692858E-4</v>
       </c>
-      <c r="D55" s="278">
+      <c r="D55" s="270">
         <v>1.3224558817292863E-3</v>
       </c>
-      <c r="E55" s="278">
+      <c r="E55" s="270">
         <v>1.9567755969446513E-3</v>
       </c>
-      <c r="F55" s="278">
+      <c r="F55" s="270">
         <v>2.5908945669240349E-3</v>
       </c>
-      <c r="G55" s="278">
+      <c r="G55" s="270">
         <v>3.2248128869481136E-3</v>
       </c>
-      <c r="H55" s="278">
+      <c r="H55" s="270">
         <v>3.8585306522372744E-3</v>
       </c>
-      <c r="I55" s="278">
+      <c r="I55" s="270">
         <v>4.4920479579516632E-3</v>
       </c>
-      <c r="J55" s="278">
+      <c r="J55" s="270">
         <v>5.1253648991912339E-3</v>
       </c>
-      <c r="K55" s="278">
+      <c r="K55" s="270">
         <v>5.7584815709957942E-3</v>
       </c>
-      <c r="L55" s="278">
+      <c r="L55" s="270">
         <v>6.3913980683450514E-3</v>
       </c>
-      <c r="M55" s="278">
+      <c r="M55" s="270">
         <v>1.6231383162068E-2</v>
       </c>
-      <c r="N55" s="278">
+      <c r="N55" s="270">
         <v>2.6023110205325765E-2</v>
       </c>
-      <c r="O55" s="278">
+      <c r="O55" s="270">
         <v>3.576693333627104E-2</v>
       </c>
-      <c r="P55" s="278">
+      <c r="P55" s="270">
         <v>4.546320323642291E-2</v>
       </c>
-      <c r="Q55" s="278">
+      <c r="Q55" s="270">
         <v>5.5112267172738066E-2</v>
       </c>
-      <c r="R55" s="278">
+      <c r="R55" s="270">
         <v>6.4714469039069161E-2</v>
       </c>
-      <c r="S55" s="278">
+      <c r="S55" s="270">
         <v>7.4270149397020507E-2</v>
       </c>
-      <c r="T55" s="278">
+      <c r="T55" s="270">
         <v>8.3779645516211296E-2</v>
       </c>
-      <c r="U55" s="278">
+      <c r="U55" s="270">
         <v>9.3243291413956611E-2</v>
       </c>
-      <c r="V55" s="278">
+      <c r="V55" s="270">
         <v>0.10266141789437581</v>
       </c>
-      <c r="W55" s="278">
+      <c r="W55" s="270">
         <v>0.1135689512148802</v>
       </c>
-      <c r="X55" s="278">
+      <c r="X55" s="270">
         <v>0.12441574637303589</v>
       </c>
-      <c r="Y55" s="278">
+      <c r="Y55" s="270">
         <v>0.13520230928728549</v>
       </c>
-      <c r="Z55" s="278">
+      <c r="Z55" s="270">
         <v>0.14592914027289947</v>
       </c>
-      <c r="AA55" s="278">
+      <c r="AA55" s="270">
         <v>0.15659673411933259</v>
       </c>
-      <c r="AB55" s="278">
+      <c r="AB55" s="270">
         <v>0.16720558016630246</v>
       </c>
-      <c r="AC55" s="278">
+      <c r="AC55" s="270">
         <v>0.17775616237861439</v>
       </c>
-      <c r="AD55" s="278">
+      <c r="AD55" s="270">
         <v>0.18824895941975692</v>
       </c>
-      <c r="AE55" s="278">
+      <c r="AE55" s="270">
         <v>0.19868444472429142</v>
       </c>
-      <c r="AF55" s="278">
+      <c r="AF55" s="270">
         <v>0.20906308656905875</v>
       </c>
     </row>
@@ -19839,233 +19834,233 @@
       <c r="A56" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="B56" s="278">
+      <c r="B56" s="270">
         <v>0.99994678616583377</v>
       </c>
-      <c r="C56" s="278">
+      <c r="C56" s="270">
         <v>0.99931206467406297</v>
       </c>
-      <c r="D56" s="278">
+      <c r="D56" s="270">
         <v>0.99867754411827081</v>
       </c>
-      <c r="E56" s="278">
+      <c r="E56" s="270">
         <v>0.99804322440305537</v>
       </c>
-      <c r="F56" s="278">
+      <c r="F56" s="270">
         <v>0.99740910543307593</v>
       </c>
-      <c r="G56" s="278">
+      <c r="G56" s="270">
         <v>0.99677518711305191</v>
       </c>
-      <c r="H56" s="278">
+      <c r="H56" s="270">
         <v>0.99614146934776271</v>
       </c>
-      <c r="I56" s="278">
+      <c r="I56" s="270">
         <v>0.99550795204204823</v>
       </c>
-      <c r="J56" s="278">
+      <c r="J56" s="270">
         <v>0.99487463510080876</v>
       </c>
-      <c r="K56" s="278">
+      <c r="K56" s="270">
         <v>0.99424151842900421</v>
       </c>
-      <c r="L56" s="278">
+      <c r="L56" s="270">
         <v>0.9936086019316549</v>
       </c>
-      <c r="M56" s="278">
+      <c r="M56" s="270">
         <v>0.98376861683793204</v>
       </c>
-      <c r="N56" s="278">
+      <c r="N56" s="270">
         <v>0.97397688979467434</v>
       </c>
-      <c r="O56" s="278">
+      <c r="O56" s="270">
         <v>0.96423306666372899</v>
       </c>
-      <c r="P56" s="278">
+      <c r="P56" s="270">
         <v>0.95453679676357717</v>
       </c>
-      <c r="Q56" s="278">
+      <c r="Q56" s="270">
         <v>0.94488773282726191</v>
       </c>
-      <c r="R56" s="278">
+      <c r="R56" s="270">
         <v>0.93528553096093092</v>
       </c>
-      <c r="S56" s="278">
+      <c r="S56" s="270">
         <v>0.92572985060297941</v>
       </c>
-      <c r="T56" s="278">
+      <c r="T56" s="270">
         <v>0.91622035448378869</v>
       </c>
-      <c r="U56" s="278">
+      <c r="U56" s="270">
         <v>0.90675670858604329</v>
       </c>
-      <c r="V56" s="278">
+      <c r="V56" s="270">
         <v>0.89733858210562423</v>
       </c>
-      <c r="W56" s="278">
+      <c r="W56" s="270">
         <v>0.88643104878511969</v>
       </c>
-      <c r="X56" s="278">
+      <c r="X56" s="270">
         <v>0.87558425362696402</v>
       </c>
-      <c r="Y56" s="278">
+      <c r="Y56" s="270">
         <v>0.86479769071271451</v>
       </c>
-      <c r="Z56" s="278">
+      <c r="Z56" s="270">
         <v>0.85407085972710062</v>
       </c>
-      <c r="AA56" s="278">
+      <c r="AA56" s="270">
         <v>0.84340326588066739</v>
       </c>
-      <c r="AB56" s="278">
+      <c r="AB56" s="270">
         <v>0.83279441983369762</v>
       </c>
-      <c r="AC56" s="278">
+      <c r="AC56" s="270">
         <v>0.82224383762138564</v>
       </c>
-      <c r="AD56" s="278">
+      <c r="AD56" s="270">
         <v>0.81175104058024306</v>
       </c>
-      <c r="AE56" s="278">
+      <c r="AE56" s="270">
         <v>0.80131555527570864</v>
       </c>
-      <c r="AF56" s="278">
+      <c r="AF56" s="270">
         <v>0.79093691343094119</v>
       </c>
     </row>
     <row r="58" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A58" s="277" t="s">
+      <c r="A58" s="269" t="s">
         <v>385</v>
       </c>
       <c r="C58" s="97"/>
     </row>
     <row r="59" spans="1:34" x14ac:dyDescent="0.35">
       <c r="C59">
-        <f t="shared" ref="C59:AH59" si="5">C50</f>
+        <f t="shared" ref="C59:AH59" si="4">C50</f>
         <v>2019</v>
       </c>
       <c r="D59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2020</v>
       </c>
       <c r="E59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2021</v>
       </c>
       <c r="F59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2022</v>
       </c>
       <c r="G59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2023</v>
       </c>
       <c r="H59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2024</v>
       </c>
       <c r="I59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2025</v>
       </c>
       <c r="J59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2026</v>
       </c>
       <c r="K59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2027</v>
       </c>
       <c r="L59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2028</v>
       </c>
       <c r="M59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2029</v>
       </c>
       <c r="N59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2030</v>
       </c>
       <c r="O59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2031</v>
       </c>
       <c r="P59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2032</v>
       </c>
       <c r="Q59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2033</v>
       </c>
       <c r="R59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2034</v>
       </c>
       <c r="S59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2035</v>
       </c>
       <c r="T59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2036</v>
       </c>
       <c r="U59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2037</v>
       </c>
       <c r="V59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2038</v>
       </c>
       <c r="W59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2039</v>
       </c>
       <c r="X59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2040</v>
       </c>
       <c r="Y59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2041</v>
       </c>
       <c r="Z59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2042</v>
       </c>
       <c r="AA59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2043</v>
       </c>
       <c r="AB59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2044</v>
       </c>
       <c r="AC59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2045</v>
       </c>
       <c r="AD59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2046</v>
       </c>
       <c r="AE59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2047</v>
       </c>
       <c r="AF59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2048</v>
       </c>
       <c r="AG59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2049</v>
       </c>
       <c r="AH59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2050</v>
       </c>
     </row>
@@ -20085,123 +20080,123 @@
         <v>92875896103395.922</v>
       </c>
       <c r="E60">
-        <f t="shared" ref="E60:AH60" si="6">E44/$A$69*C56</f>
+        <f t="shared" ref="E60:AH60" si="5">E44/$A$69*C56</f>
         <v>92629566885328.219</v>
       </c>
       <c r="F60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>92034165932313.172</v>
       </c>
       <c r="G60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>91296368798764.578</v>
       </c>
       <c r="H60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>90380958678748.375</v>
       </c>
       <c r="I60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>89583463573621.922</v>
       </c>
       <c r="J60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>89074759701332.781</v>
       </c>
       <c r="K60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>88349879469480.094</v>
       </c>
       <c r="L60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>87977530086883.016</v>
       </c>
       <c r="M60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>87542292906353.094</v>
       </c>
       <c r="N60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>86915186092376.188</v>
       </c>
       <c r="O60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>85816353759257.156</v>
       </c>
       <c r="P60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>84606700144573.906</v>
       </c>
       <c r="Q60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>83283149097788.719</v>
       </c>
       <c r="R60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>81975136335499.734</v>
       </c>
       <c r="S60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>80312820366073.906</v>
       </c>
       <c r="T60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>79235091473000.5</v>
       </c>
       <c r="U60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>77758096395745.031</v>
       </c>
       <c r="V60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>76415752890403</v>
       </c>
       <c r="W60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>75054028936018.344</v>
       </c>
       <c r="X60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>73678521639098.797</v>
       </c>
       <c r="Y60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>72007905134253.938</v>
       </c>
       <c r="Z60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>70565408112553.281</v>
       </c>
       <c r="AA60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>68976062434342.617</v>
       </c>
       <c r="AB60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>67528259483084.133</v>
       </c>
       <c r="AC60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>66197729228535.602</v>
       </c>
       <c r="AD60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>64920342392482.055</v>
       </c>
       <c r="AE60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>63487792853979.711</v>
       </c>
       <c r="AF60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>62213886843710.195</v>
       </c>
       <c r="AG60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>60946265240823.625</v>
       </c>
       <c r="AH60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>59565547543108.453</v>
       </c>
     </row>
@@ -20221,123 +20216,123 @@
         <v>829657309022245.5</v>
       </c>
       <c r="E61">
-        <f t="shared" ref="E61:AH61" si="7">E52/$A$69*C56</f>
+        <f t="shared" ref="E61:AH61" si="6">E52/$A$69*C56</f>
         <v>835214518601608.75</v>
       </c>
       <c r="F61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>840399358855612.88</v>
       </c>
       <c r="G61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>843523349922873.63</v>
       </c>
       <c r="H61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>844572161536242.38</v>
       </c>
       <c r="I61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>846635166629183.75</v>
       </c>
       <c r="J61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>849682140974467.75</v>
       </c>
       <c r="K61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>852112986006920.25</v>
       </c>
       <c r="L61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>854968289473391</v>
       </c>
       <c r="M61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>857079626875687.38</v>
       </c>
       <c r="N61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>857811134765694.88</v>
       </c>
       <c r="O61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>852367047971016.13</v>
       </c>
       <c r="P61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>845927897511548.88</v>
       </c>
       <c r="Q61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>839210737074747</v>
       </c>
       <c r="R61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>832029139894014.25</v>
       </c>
       <c r="S61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>823522469040744.5</v>
       </c>
       <c r="T61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>817533676391561.5</v>
       </c>
       <c r="U61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>810248127758334.38</v>
       </c>
       <c r="V61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>803557010385176.63</v>
       </c>
       <c r="W61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>796538257052109.25</v>
       </c>
       <c r="X61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>789762028354424.5</v>
       </c>
       <c r="Y61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>781166425694781.13</v>
       </c>
       <c r="Z61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>773829999955077.25</v>
       </c>
       <c r="AA61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>765302221845296</v>
       </c>
       <c r="AB61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>757571381024720.5</v>
       </c>
       <c r="AC61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>749134490843442.13</v>
       </c>
       <c r="AD61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>741768820749807.38</v>
       </c>
       <c r="AE61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>733735230850786.63</v>
       </c>
       <c r="AF61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>726100675589404.25</v>
       </c>
       <c r="AG61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>718079929166449.5</v>
       </c>
       <c r="AH61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>709655103570678</v>
       </c>
     </row>
@@ -20348,134 +20343,137 @@
       <c r="B62" t="s">
         <v>366</v>
       </c>
-      <c r="C62" s="279">
+      <c r="C62" s="271">
         <f>C45/$A$71</f>
         <v>119564270152505.45</v>
       </c>
-      <c r="D62" s="279">
+      <c r="D62" s="271">
         <f>D45/$A$71*B56</f>
         <v>118881147012346.78</v>
       </c>
-      <c r="E62" s="279">
-        <f t="shared" ref="E62:AH62" si="8">E45/$A$71*C56</f>
+      <c r="E62" s="271">
+        <f t="shared" ref="E62:AH62" si="7">E45/$A$71*C56</f>
         <v>118565845613220.14</v>
       </c>
-      <c r="F62" s="279">
-        <f t="shared" si="8"/>
+      <c r="F62" s="271">
+        <f t="shared" si="7"/>
         <v>117803732393360.89</v>
       </c>
-      <c r="G62" s="279">
-        <f t="shared" si="8"/>
+      <c r="G62" s="271">
+        <f t="shared" si="7"/>
         <v>116859352062418.69</v>
       </c>
-      <c r="H62" s="279">
-        <f t="shared" si="8"/>
+      <c r="H62" s="271">
+        <f t="shared" si="7"/>
         <v>115687627108797.97</v>
       </c>
-      <c r="I62" s="279">
-        <f t="shared" si="8"/>
+      <c r="I62" s="271">
+        <f t="shared" si="7"/>
         <v>114666833374236.11</v>
       </c>
-      <c r="J62" s="279">
-        <f t="shared" si="8"/>
+      <c r="J62" s="271">
+        <f t="shared" si="7"/>
         <v>114015692417706.03</v>
       </c>
-      <c r="K62" s="279">
-        <f t="shared" si="8"/>
+      <c r="K62" s="271">
+        <f t="shared" si="7"/>
         <v>113087845720934.59</v>
       </c>
-      <c r="L62" s="279">
-        <f t="shared" si="8"/>
+      <c r="L62" s="271">
+        <f t="shared" si="7"/>
         <v>112611238511210.31</v>
       </c>
-      <c r="M62" s="279">
-        <f t="shared" si="8"/>
+      <c r="M62" s="271">
+        <f t="shared" si="7"/>
         <v>112054134920132.02</v>
       </c>
-      <c r="N62" s="279">
-        <f t="shared" si="8"/>
+      <c r="N62" s="271">
+        <f t="shared" si="7"/>
         <v>111251438198241.58</v>
       </c>
-      <c r="O62" s="279">
-        <f t="shared" si="8"/>
+      <c r="O62" s="271">
+        <f t="shared" si="7"/>
         <v>109844932811849.22</v>
       </c>
-      <c r="P62" s="279">
-        <f t="shared" si="8"/>
+      <c r="P62" s="271">
+        <f t="shared" si="7"/>
         <v>108296576185054.69</v>
       </c>
-      <c r="Q62" s="279">
-        <f t="shared" si="8"/>
+      <c r="Q62" s="271">
+        <f t="shared" si="7"/>
         <v>106602430845169.64</v>
       </c>
-      <c r="R62" s="279">
-        <f t="shared" si="8"/>
+      <c r="R62" s="271">
+        <f t="shared" si="7"/>
         <v>104928174509439.75</v>
       </c>
-      <c r="S62" s="279">
-        <f t="shared" si="8"/>
+      <c r="S62" s="271">
+        <f t="shared" si="7"/>
         <v>102800410068574.69</v>
       </c>
-      <c r="T62" s="279">
-        <f t="shared" si="8"/>
+      <c r="T62" s="271">
+        <f t="shared" si="7"/>
         <v>101420917085440.73</v>
       </c>
-      <c r="U62" s="279">
-        <f t="shared" si="8"/>
+      <c r="U62" s="271">
+        <f t="shared" si="7"/>
         <v>99530363386553.75</v>
       </c>
-      <c r="V62" s="279">
-        <f t="shared" si="8"/>
+      <c r="V62" s="271">
+        <f t="shared" si="7"/>
         <v>97812163699715.938</v>
       </c>
-      <c r="W62" s="279">
-        <f t="shared" si="8"/>
+      <c r="W62" s="271">
+        <f t="shared" si="7"/>
         <v>96069157038103.578</v>
       </c>
-      <c r="X62" s="279">
-        <f t="shared" si="8"/>
+      <c r="X62" s="271">
+        <f t="shared" si="7"/>
         <v>94308507698046.563</v>
       </c>
-      <c r="Y62" s="279">
-        <f t="shared" si="8"/>
+      <c r="Y62" s="271">
+        <f t="shared" si="7"/>
         <v>92170118571845.141</v>
       </c>
-      <c r="Z62" s="279">
-        <f t="shared" si="8"/>
+      <c r="Z62" s="271">
+        <f t="shared" si="7"/>
         <v>90323722384068.266</v>
       </c>
-      <c r="AA62" s="279">
-        <f t="shared" si="8"/>
+      <c r="AA62" s="271">
+        <f t="shared" si="7"/>
         <v>88289359915958.641</v>
       </c>
-      <c r="AB62" s="279">
-        <f t="shared" si="8"/>
+      <c r="AB62" s="271">
+        <f t="shared" si="7"/>
         <v>86436172138347.781</v>
       </c>
-      <c r="AC62" s="279">
-        <f t="shared" si="8"/>
+      <c r="AC62" s="271">
+        <f t="shared" si="7"/>
         <v>84733093412525.641</v>
       </c>
-      <c r="AD62" s="279">
-        <f t="shared" si="8"/>
+      <c r="AD62" s="271">
+        <f t="shared" si="7"/>
         <v>83098038262377.063</v>
       </c>
-      <c r="AE62" s="279">
-        <f t="shared" si="8"/>
+      <c r="AE62" s="271">
+        <f t="shared" si="7"/>
         <v>81264374853094.094</v>
       </c>
-      <c r="AF62" s="279">
-        <f t="shared" si="8"/>
+      <c r="AF62" s="271">
+        <f t="shared" si="7"/>
         <v>79633775159949.109</v>
       </c>
-      <c r="AG62" s="279">
-        <f t="shared" si="8"/>
+      <c r="AG62" s="271">
+        <f t="shared" si="7"/>
         <v>78011219508254.297</v>
       </c>
-      <c r="AH62" s="279">
-        <f t="shared" si="8"/>
+      <c r="AH62" s="271">
+        <f t="shared" si="7"/>
         <v>76243900855178.875</v>
       </c>
+    </row>
+    <row r="63" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="C63" s="271"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" s="259" t="s">
@@ -20530,7 +20528,7 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A70" s="280">
+      <c r="A70" s="272">
         <v>0.453592</v>
       </c>
       <c r="B70" t="s">
@@ -20549,10 +20547,10 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A72" s="281"/>
-    </row>
-    <row r="73" spans="1:11" s="283" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="282" t="s">
+      <c r="A72" s="273"/>
+    </row>
+    <row r="73" spans="1:11" s="275" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="274" t="s">
         <v>399</v>
       </c>
     </row>
@@ -20639,7 +20637,7 @@
   <dimension ref="A1:AF16"/>
   <sheetViews>
     <sheetView topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20879,128 +20877,128 @@
         <v>151</v>
       </c>
       <c r="B3" s="86">
-        <f>(1-B2)*'TYNDP Data'!$B24*SUM('(BIFUbC) Historical Production'!D$60:D$61)/SUM('(BIFUbC) Historical Production'!D$60:D$62)</f>
-        <v>0.66487562484988016</v>
+        <f>(1-B2)*'TYNDP Data'!$B24*SUM('(BIFUbC) Historical Production'!C43:C44,'(BIFUbC) Historical Production'!C46)/SUM('(BIFUbC) Historical Production'!C43:C46)</f>
+        <v>0.66867541162563049</v>
       </c>
       <c r="C3" s="14">
         <f>($L3-$B3)/10*(C$1-$B$1)+$B3</f>
-        <v>0.66521610875975923</v>
+        <v>0.66902990460759848</v>
       </c>
       <c r="D3" s="14">
         <f t="shared" ref="D3:K3" si="3">($L3-$B3)/10*(D$1-$B$1)+$B3</f>
-        <v>0.6655565926696384</v>
+        <v>0.66938439758956658</v>
       </c>
       <c r="E3" s="14">
         <f t="shared" si="3"/>
-        <v>0.66589707657951747</v>
+        <v>0.66973889057153457</v>
       </c>
       <c r="F3" s="14">
         <f t="shared" si="3"/>
-        <v>0.66623756048939664</v>
+        <v>0.67009338355350268</v>
       </c>
       <c r="G3" s="14">
         <f t="shared" si="3"/>
-        <v>0.6665780443992757</v>
+        <v>0.67044787653547067</v>
       </c>
       <c r="H3" s="14">
         <f t="shared" si="3"/>
-        <v>0.66691852830915477</v>
+        <v>0.67080236951743866</v>
       </c>
       <c r="I3" s="14">
         <f t="shared" si="3"/>
-        <v>0.66725901221903394</v>
+        <v>0.67115686249940676</v>
       </c>
       <c r="J3" s="14">
         <f t="shared" si="3"/>
-        <v>0.66759949612891301</v>
+        <v>0.67151135548137475</v>
       </c>
       <c r="K3" s="14">
         <f t="shared" si="3"/>
-        <v>0.66793998003879218</v>
+        <v>0.67186584846334285</v>
       </c>
       <c r="L3" s="86">
-        <f>(1-L2)*'TYNDP Data'!$B24*SUM('(BIFUbC) Historical Production'!N$60:N$61)/SUM('(BIFUbC) Historical Production'!N$60:N$62)</f>
-        <v>0.66828046394867124</v>
+        <f>(1-L2)*'TYNDP Data'!$B24*SUM('(BIFUbC) Historical Production'!M43:M44,'(BIFUbC) Historical Production'!M46)/SUM('(BIFUbC) Historical Production'!M43:M46)</f>
+        <v>0.67222034144531084</v>
       </c>
       <c r="M3" s="14">
         <f>($V3-$L3)/10*(M$1-$L$1)+$L3</f>
-        <v>0.66376869318731835</v>
+        <v>0.66764727342992869</v>
       </c>
       <c r="N3" s="14">
         <f t="shared" ref="N3:U3" si="4">($V3-$L3)/10*(N$1-$L$1)+$L3</f>
-        <v>0.65925692242596556</v>
+        <v>0.66307420541454654</v>
       </c>
       <c r="O3" s="14">
         <f t="shared" si="4"/>
-        <v>0.65474515166461267</v>
+        <v>0.65850113739916427</v>
       </c>
       <c r="P3" s="14">
         <f t="shared" si="4"/>
-        <v>0.65023338090325988</v>
+        <v>0.65392806938378212</v>
       </c>
       <c r="Q3" s="14">
         <f t="shared" si="4"/>
-        <v>0.64572161014190699</v>
+        <v>0.64935500136839996</v>
       </c>
       <c r="R3" s="14">
         <f t="shared" si="4"/>
-        <v>0.64120983938055409</v>
+        <v>0.64478193335301781</v>
       </c>
       <c r="S3" s="14">
         <f t="shared" si="4"/>
-        <v>0.63669806861920131</v>
+        <v>0.64020886533763566</v>
       </c>
       <c r="T3" s="14">
         <f t="shared" si="4"/>
-        <v>0.63218629785784841</v>
+        <v>0.63563579732225339</v>
       </c>
       <c r="U3" s="14">
         <f t="shared" si="4"/>
-        <v>0.62767452709649563</v>
+        <v>0.63106272930687124</v>
       </c>
       <c r="V3" s="86">
-        <f>(1-V2)*'TYNDP Data'!$B24*SUM('(BIFUbC) Historical Production'!X$60:X$61)/SUM('(BIFUbC) Historical Production'!X$60:X$62)</f>
-        <v>0.62316275633514273</v>
+        <f>(1-V2)*'TYNDP Data'!$B24*SUM('(BIFUbC) Historical Production'!W43:W44,'(BIFUbC) Historical Production'!W46)/SUM('(BIFUbC) Historical Production'!W43:W46)</f>
+        <v>0.62648966129148909</v>
       </c>
       <c r="W3" s="14">
         <f>($AF3-$V3)/10*(W$1-$V$1)+$V3</f>
-        <v>0.61783064381810471</v>
+        <v>0.62109770793412089</v>
       </c>
       <c r="X3" s="14">
         <f t="shared" ref="X3:AE3" si="5">($AF3-$V3)/10*(X$1-$V$1)+$V3</f>
-        <v>0.61249853130106657</v>
+        <v>0.61570575457675258</v>
       </c>
       <c r="Y3" s="14">
         <f t="shared" si="5"/>
-        <v>0.60716641878402855</v>
+        <v>0.61031380121938428</v>
       </c>
       <c r="Z3" s="14">
         <f t="shared" si="5"/>
-        <v>0.60183430626699053</v>
+        <v>0.60492184786201608</v>
       </c>
       <c r="AA3" s="14">
         <f t="shared" si="5"/>
-        <v>0.59650219374995239</v>
+        <v>0.59952989450464789</v>
       </c>
       <c r="AB3" s="14">
         <f t="shared" si="5"/>
-        <v>0.59117008123291437</v>
+        <v>0.59413794114727958</v>
       </c>
       <c r="AC3" s="14">
         <f t="shared" si="5"/>
-        <v>0.58583796871587634</v>
+        <v>0.58874598778991127</v>
       </c>
       <c r="AD3" s="14">
         <f t="shared" si="5"/>
-        <v>0.58050585619883832</v>
+        <v>0.58335403443254308</v>
       </c>
       <c r="AE3" s="14">
         <f t="shared" si="5"/>
-        <v>0.57517374368180019</v>
+        <v>0.57796208107517488</v>
       </c>
       <c r="AF3" s="86">
-        <f>(1-AF2)*'TYNDP Data'!$B24*SUM('(BIFUbC) Historical Production'!AH$60:AH$61)/SUM('(BIFUbC) Historical Production'!AH$60:AH$62)</f>
-        <v>0.56984163116476216</v>
+        <f>(1-AF2)*'TYNDP Data'!$B24*SUM('(BIFUbC) Historical Production'!AG43:AG44,'(BIFUbC) Historical Production'!AG46)/SUM('(BIFUbC) Historical Production'!AG43:AG46)</f>
+        <v>0.57257012771780658</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.35">
@@ -21204,128 +21202,128 @@
         <v>161</v>
       </c>
       <c r="B6" s="86">
-        <f>(1-B2)*'TYNDP Data'!$B24*SUM('(BIFUbC) Historical Production'!D$62:D$62)/SUM('(BIFUbC) Historical Production'!D$60:D$62)</f>
-        <v>8.5678408607460135E-2</v>
+        <f>(1-B2)*'TYNDP Data'!$B24*'(BIFUbC) Historical Production'!D45/SUM('(BIFUbC) Historical Production'!D43:D46)</f>
+        <v>8.0900701973206035E-2</v>
       </c>
       <c r="C6" s="14">
         <f>($L6-$B6)/10*(C$1-$B$1)+$B6</f>
-        <v>8.4980271500341958E-2</v>
+        <v>8.0237381387333398E-2</v>
       </c>
       <c r="D6" s="14">
         <f t="shared" ref="D6:K6" si="6">($L6-$B6)/10*(D$1-$B$1)+$B6</f>
-        <v>8.4282134393223782E-2</v>
+        <v>7.9574060801460747E-2</v>
       </c>
       <c r="E6" s="14">
         <f t="shared" si="6"/>
-        <v>8.3583997286105619E-2</v>
+        <v>7.891074021558811E-2</v>
       </c>
       <c r="F6" s="14">
         <f t="shared" si="6"/>
-        <v>8.2885860178987442E-2</v>
+        <v>7.8247419629715459E-2</v>
       </c>
       <c r="G6" s="14">
         <f t="shared" si="6"/>
-        <v>8.2187723071869265E-2</v>
+        <v>7.7584099043842822E-2</v>
       </c>
       <c r="H6" s="14">
         <f t="shared" si="6"/>
-        <v>8.1489585964751088E-2</v>
+        <v>7.6920778457970185E-2</v>
       </c>
       <c r="I6" s="14">
         <f t="shared" si="6"/>
-        <v>8.0791448857632911E-2</v>
+        <v>7.6257457872097534E-2</v>
       </c>
       <c r="J6" s="14">
         <f t="shared" si="6"/>
-        <v>8.0093311750514748E-2</v>
+        <v>7.5594137286224897E-2</v>
       </c>
       <c r="K6" s="14">
         <f t="shared" si="6"/>
-        <v>7.9395174643396571E-2</v>
+        <v>7.4930816700352246E-2</v>
       </c>
       <c r="L6" s="86">
-        <f>(1-L2)*'TYNDP Data'!$B24*SUM('(BIFUbC) Historical Production'!N$62:N$62)/SUM('(BIFUbC) Historical Production'!N$60:N$62)</f>
-        <v>7.8697037536278394E-2</v>
+        <f>(1-L2)*'TYNDP Data'!$B24*'(BIFUbC) Historical Production'!N45/SUM('(BIFUbC) Historical Production'!N43:N46)</f>
+        <v>7.4267496114479609E-2</v>
       </c>
       <c r="M6" s="14">
         <f>($V6-$L6)/10*(M$1-$L$1)+$L6</f>
-        <v>7.7633772234424636E-2</v>
+        <v>7.3261296587908642E-2</v>
       </c>
       <c r="N6" s="14">
         <f t="shared" ref="N6:U6" si="7">($V6-$L6)/10*(N$1-$L$1)+$L6</f>
-        <v>7.6570506932570864E-2</v>
+        <v>7.2255097061337689E-2</v>
       </c>
       <c r="O6" s="14">
         <f t="shared" si="7"/>
-        <v>7.5507241630717092E-2</v>
+        <v>7.1248897534766722E-2</v>
       </c>
       <c r="P6" s="14">
         <f t="shared" si="7"/>
-        <v>7.4443976328863334E-2</v>
+        <v>7.024269800819577E-2</v>
       </c>
       <c r="Q6" s="14">
         <f t="shared" si="7"/>
-        <v>7.3380711027009576E-2</v>
+        <v>6.9236498481624803E-2</v>
       </c>
       <c r="R6" s="14">
         <f t="shared" si="7"/>
-        <v>7.2317445725155804E-2</v>
+        <v>6.8230298955053836E-2</v>
       </c>
       <c r="S6" s="14">
         <f t="shared" si="7"/>
-        <v>7.1254180423302033E-2</v>
+        <v>6.7224099428482884E-2</v>
       </c>
       <c r="T6" s="14">
         <f t="shared" si="7"/>
-        <v>7.0190915121448275E-2</v>
+        <v>6.6217899901911917E-2</v>
       </c>
       <c r="U6" s="14">
         <f t="shared" si="7"/>
-        <v>6.9127649819594517E-2</v>
+        <v>6.5211700375340964E-2</v>
       </c>
       <c r="V6" s="86">
-        <f>(1-V2)*'TYNDP Data'!$B24*SUM('(BIFUbC) Historical Production'!X$62:X$62)/SUM('(BIFUbC) Historical Production'!X$60:X$62)</f>
-        <v>6.8064384517740745E-2</v>
+        <f>(1-V2)*'TYNDP Data'!$B24*'(BIFUbC) Historical Production'!X45/SUM('(BIFUbC) Historical Production'!X43:X46)</f>
+        <v>6.4205500848769997E-2</v>
       </c>
       <c r="W6" s="14">
         <f>($AF6-$V6)/10*(W$1-$V$1)+$V6</f>
-        <v>6.6906123707423756E-2</v>
+        <v>6.3110131315251339E-2</v>
       </c>
       <c r="X6" s="14">
         <f t="shared" ref="X6:AE6" si="8">($AF6-$V6)/10*(X$1-$V$1)+$V6</f>
-        <v>6.5747862897106768E-2</v>
+        <v>6.2014761781732673E-2</v>
       </c>
       <c r="Y6" s="14">
         <f t="shared" si="8"/>
-        <v>6.4589602086789794E-2</v>
+        <v>6.0919392248214008E-2</v>
       </c>
       <c r="Z6" s="14">
         <f t="shared" si="8"/>
-        <v>6.3431341276472805E-2</v>
+        <v>5.9824022714695349E-2</v>
       </c>
       <c r="AA6" s="14">
         <f t="shared" si="8"/>
-        <v>6.2273080466155817E-2</v>
+        <v>5.8728653181176683E-2</v>
       </c>
       <c r="AB6" s="14">
         <f t="shared" si="8"/>
-        <v>6.1114819655838828E-2</v>
+        <v>5.7633283647658018E-2</v>
       </c>
       <c r="AC6" s="14">
         <f t="shared" si="8"/>
-        <v>5.9956558845521847E-2</v>
+        <v>5.6537914114139359E-2</v>
       </c>
       <c r="AD6" s="14">
         <f t="shared" si="8"/>
-        <v>5.8798298035204859E-2</v>
+        <v>5.5442544580620694E-2</v>
       </c>
       <c r="AE6" s="14">
         <f t="shared" si="8"/>
-        <v>5.7640037224887877E-2</v>
+        <v>5.4347175047102035E-2</v>
       </c>
       <c r="AF6" s="86">
-        <f>(1-AF2)*'TYNDP Data'!$B24*SUM('(BIFUbC) Historical Production'!AH$62:AH$62)/SUM('(BIFUbC) Historical Production'!AH$60:AH$62)</f>
-        <v>5.6481776414570889E-2</v>
+        <f>(1-AF2)*'TYNDP Data'!$B24*'(BIFUbC) Historical Production'!AH45/SUM('(BIFUbC) Historical Production'!AH43:AH46)</f>
+        <v>5.325180551358337E-2</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.35">
@@ -21463,127 +21461,127 @@
       </c>
       <c r="B9" s="14">
         <f>SUM(B2:B7)</f>
-        <v>1</v>
+        <v>0.9990220801414964</v>
       </c>
       <c r="C9" s="14">
         <f t="shared" ref="C9:AF9" si="12">SUM(C2:C7)</f>
-        <v>1</v>
+        <v>0.99907090573483071</v>
       </c>
       <c r="D9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99911973132816523</v>
       </c>
       <c r="E9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99916855692149964</v>
       </c>
       <c r="F9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99921738251483416</v>
       </c>
       <c r="G9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99926620810816846</v>
       </c>
       <c r="H9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99931503370150288</v>
       </c>
       <c r="I9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99936385929483751</v>
       </c>
       <c r="J9" s="14">
         <f t="shared" si="12"/>
-        <v>0.99999999999999989</v>
+        <v>0.99941268488817181</v>
       </c>
       <c r="K9" s="14">
         <f t="shared" si="12"/>
-        <v>0.99999999999999989</v>
+        <v>0.99946151048150633</v>
       </c>
       <c r="L9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99951033607484074</v>
       </c>
       <c r="M9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99950610459609424</v>
       </c>
       <c r="N9" s="14">
         <f t="shared" si="12"/>
-        <v>0.99999999999999989</v>
+        <v>0.99950187311734773</v>
       </c>
       <c r="O9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99949764163860122</v>
       </c>
       <c r="P9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99949341015985471</v>
       </c>
       <c r="Q9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.9994891786811082</v>
       </c>
       <c r="R9" s="14">
         <f t="shared" si="12"/>
-        <v>0.99999999999999989</v>
+        <v>0.9994849472023617</v>
       </c>
       <c r="S9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99948071572361519</v>
       </c>
       <c r="T9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99947648424486868</v>
       </c>
       <c r="U9" s="14">
         <f t="shared" si="12"/>
-        <v>1.0000000000000002</v>
+        <v>0.99947225276612217</v>
       </c>
       <c r="V9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99946802128737566</v>
       </c>
       <c r="W9" s="14">
         <f>SUM(W2:W7)</f>
-        <v>1</v>
+        <v>0.99947107172384386</v>
       </c>
       <c r="X9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99947412216031206</v>
       </c>
       <c r="Y9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99947717259677993</v>
       </c>
       <c r="Z9" s="14">
         <f t="shared" si="12"/>
-        <v>1.0000000000000002</v>
+        <v>0.99948022303324824</v>
       </c>
       <c r="AA9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99948327346971644</v>
       </c>
       <c r="AB9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99948632390618442</v>
       </c>
       <c r="AC9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.9994893743426525</v>
       </c>
       <c r="AD9" s="14">
         <f t="shared" si="12"/>
-        <v>1.0000000000000002</v>
+        <v>0.99949242477912081</v>
       </c>
       <c r="AE9" s="14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.99949547521558901</v>
       </c>
       <c r="AF9" s="14">
         <f t="shared" si="12"/>
-        <v>1.0000000000000002</v>
+        <v>0.99949852565205699</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.35">
@@ -21619,7 +21617,7 @@
   <dimension ref="A1:AF8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21731,127 +21729,127 @@
       </c>
       <c r="B2" s="263">
         <f>Calculations!B2/SUM(Calculations!B$2:B$6)</f>
-        <v>5.3213834166182343E-5</v>
+        <v>5.3283254858002796E-5</v>
       </c>
       <c r="C2" s="263">
         <f>Calculations!C2/SUM(Calculations!C$2:C$6)</f>
-        <v>6.8793532593692868E-4</v>
+        <v>6.8878778077474635E-4</v>
       </c>
       <c r="D2" s="263">
         <f>Calculations!D2/SUM(Calculations!D$2:D$6)</f>
-        <v>1.3224558817292863E-3</v>
+        <v>1.324008137625256E-3</v>
       </c>
       <c r="E2" s="263">
         <f>Calculations!E2/SUM(Calculations!E$2:E$6)</f>
-        <v>1.9567755969446513E-3</v>
+        <v>1.9589445159683828E-3</v>
       </c>
       <c r="F2" s="263">
         <f>Calculations!F2/SUM(Calculations!F$2:F$6)</f>
-        <v>2.5908945669240345E-3</v>
+        <v>2.5935971061926332E-3</v>
       </c>
       <c r="G2" s="263">
         <f>Calculations!G2/SUM(Calculations!G$2:G$6)</f>
-        <v>3.2248128869481136E-3</v>
+        <v>3.2279660985163649E-3</v>
       </c>
       <c r="H2" s="263">
         <f>Calculations!H2/SUM(Calculations!H$2:H$6)</f>
-        <v>3.8585306522372748E-3</v>
+        <v>3.8620516829879687E-3</v>
       </c>
       <c r="I2" s="263">
         <f>Calculations!I2/SUM(Calculations!I$2:I$6)</f>
-        <v>4.4920479579516632E-3</v>
+        <v>4.4958540494860659E-3</v>
       </c>
       <c r="J2" s="263">
         <f>Calculations!J2/SUM(Calculations!J$2:J$6)</f>
-        <v>5.1253648991912348E-3</v>
+        <v>5.1293733877196979E-3</v>
       </c>
       <c r="K2" s="263">
         <f>Calculations!K2/SUM(Calculations!K$2:K$6)</f>
-        <v>5.7584815709957942E-3</v>
+        <v>5.7626098872285043E-3</v>
       </c>
       <c r="L2" s="263">
         <f>Calculations!L2/SUM(Calculations!L$2:L$6)</f>
-        <v>6.3913980683450514E-3</v>
+        <v>6.3955637373829281E-3</v>
       </c>
       <c r="M2" s="263">
         <f>Calculations!M2/SUM(Calculations!M$2:M$6)</f>
-        <v>1.6231383162068E-2</v>
+        <v>1.6242027389891937E-2</v>
       </c>
       <c r="N2" s="263">
         <f>Calculations!N2/SUM(Calculations!N$2:N$6)</f>
-        <v>2.6023110205325765E-2</v>
+        <v>2.6040279731281823E-2</v>
       </c>
       <c r="O2" s="263">
         <f>Calculations!O2/SUM(Calculations!O$2:O$6)</f>
-        <v>3.576693333627104E-2</v>
+        <v>3.5790673982898875E-2</v>
       </c>
       <c r="P2" s="263">
         <f>Calculations!P2/SUM(Calculations!P$2:P$6)</f>
-        <v>4.5463203236422903E-2</v>
+        <v>4.5493559923982567E-2</v>
       </c>
       <c r="Q2" s="263">
         <f>Calculations!Q2/SUM(Calculations!Q$2:Q$6)</f>
-        <v>5.5112267172738059E-2</v>
+        <v>5.5149283933492305E-2</v>
       </c>
       <c r="R2" s="263">
         <f>Calculations!R2/SUM(Calculations!R$2:R$6)</f>
-        <v>6.4714469039069175E-2</v>
+        <v>6.4758189031325963E-2</v>
       </c>
       <c r="S2" s="263">
         <f>Calculations!S2/SUM(Calculations!S$2:S$6)</f>
-        <v>7.4270149397020507E-2</v>
+        <v>7.4320614918940001E-2</v>
       </c>
       <c r="T2" s="263">
         <f>Calculations!T2/SUM(Calculations!T$2:T$6)</f>
-        <v>8.3779645516211296E-2</v>
+        <v>8.3836898019381864E-2</v>
       </c>
       <c r="U2" s="263">
         <f>Calculations!U2/SUM(Calculations!U$2:U$6)</f>
-        <v>9.3243291413956597E-2</v>
+        <v>9.3307371516743912E-2</v>
       </c>
       <c r="V2" s="263">
         <f>Calculations!V2/SUM(Calculations!V$2:V$6)</f>
-        <v>0.1026614178943758</v>
+        <v>0.10273236539504935</v>
       </c>
       <c r="W2" s="263">
         <f>Calculations!W2/SUM(Calculations!W$2:W$6)</f>
-        <v>0.1135689512148802</v>
+        <v>0.11364676834080144</v>
       </c>
       <c r="X2" s="263">
         <f>Calculations!X2/SUM(Calculations!X$2:X$6)</f>
-        <v>0.12441574637303589</v>
+        <v>0.124500267563244</v>
       </c>
       <c r="Y2" s="263">
         <f>Calculations!Y2/SUM(Calculations!Y$2:Y$6)</f>
-        <v>0.13520230928728549</v>
+        <v>0.13529337141953374</v>
       </c>
       <c r="Z2" s="263">
         <f>Calculations!Z2/SUM(Calculations!Z$2:Z$6)</f>
-        <v>0.14592914027289944</v>
+        <v>0.14602658262491761</v>
       </c>
       <c r="AA2" s="263">
         <f>Calculations!AA2/SUM(Calculations!AA$2:AA$6)</f>
-        <v>0.15659673411933259</v>
+        <v>0.15670039833078631</v>
       </c>
       <c r="AB2" s="263">
         <f>Calculations!AB2/SUM(Calculations!AB$2:AB$6)</f>
-        <v>0.16720558016630244</v>
+        <v>0.16731531020143495</v>
       </c>
       <c r="AC2" s="263">
         <f>Calculations!AC2/SUM(Calculations!AC$2:AC$6)</f>
-        <v>0.17775616237861436</v>
+        <v>0.17787180448955639</v>
       </c>
       <c r="AD2" s="263">
         <f>Calculations!AD2/SUM(Calculations!AD$2:AD$6)</f>
-        <v>0.18824895941975689</v>
+        <v>0.1883703621104921</v>
       </c>
       <c r="AE2" s="263">
         <f>Calculations!AE2/SUM(Calculations!AE$2:AE$6)</f>
-        <v>0.19868444472429142</v>
+        <v>0.19881145871526335</v>
       </c>
       <c r="AF2" s="263">
         <f>Calculations!AF2/SUM(Calculations!AF$2:AF$6)</f>
-        <v>0.20906308656905875</v>
+        <v>0.20919556476240689</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
@@ -21860,127 +21858,127 @@
       </c>
       <c r="B3" s="263">
         <f>Calculations!B3/SUM(Calculations!B$2:B$6)</f>
-        <v>0.88579930908655391</v>
+        <v>0.89202386561253588</v>
       </c>
       <c r="C3" s="263">
         <f>Calculations!C3/SUM(Calculations!C$2:C$6)</f>
-        <v>0.88611262409541636</v>
+        <v>0.89229717816460774</v>
       </c>
       <c r="D3" s="263">
         <f>Calculations!D3/SUM(Calculations!D$2:D$6)</f>
-        <v>0.88642583991706281</v>
+        <v>0.89257036850358817</v>
       </c>
       <c r="E3" s="263">
         <f>Calculations!E3/SUM(Calculations!E$2:E$6)</f>
-        <v>0.88673895659858526</v>
+        <v>0.89284343671143129</v>
       </c>
       <c r="F3" s="263">
         <f>Calculations!F3/SUM(Calculations!F$2:F$6)</f>
-        <v>0.88705197418704707</v>
+        <v>0.89311638287001749</v>
       </c>
       <c r="G3" s="263">
         <f>Calculations!G3/SUM(Calculations!G$2:G$6)</f>
-        <v>0.88736489272948127</v>
+        <v>0.89338920706115477</v>
       </c>
       <c r="H3" s="263">
         <f>Calculations!H3/SUM(Calculations!H$2:H$6)</f>
-        <v>0.88767771227289072</v>
+        <v>0.89366190936657708</v>
       </c>
       <c r="I3" s="263">
         <f>Calculations!I3/SUM(Calculations!I$2:I$6)</f>
-        <v>0.88799043286424917</v>
+        <v>0.8939344898679461</v>
       </c>
       <c r="J3" s="263">
         <f>Calculations!J3/SUM(Calculations!J$2:J$6)</f>
-        <v>0.88830305455050051</v>
+        <v>0.89420694864685069</v>
       </c>
       <c r="K3" s="263">
         <f>Calculations!K3/SUM(Calculations!K$2:K$6)</f>
-        <v>0.88861557737855856</v>
+        <v>0.89447928578480584</v>
       </c>
       <c r="L3" s="263">
         <f>Calculations!L3/SUM(Calculations!L$2:L$6)</f>
-        <v>0.88892800139530781</v>
+        <v>0.89475150136325488</v>
       </c>
       <c r="M3" s="263">
         <f>Calculations!M3/SUM(Calculations!M$2:M$6)</f>
-        <v>0.88075618797107325</v>
+        <v>0.88648364279587244</v>
       </c>
       <c r="N3" s="263">
         <f>Calculations!N3/SUM(Calculations!N$2:N$6)</f>
-        <v>0.87262445141492972</v>
+        <v>0.87825626620412589</v>
       </c>
       <c r="O3" s="263">
         <f>Calculations!O3/SUM(Calculations!O$2:O$6)</f>
-        <v>0.86453249762572926</v>
+        <v>0.87006907499583375</v>
       </c>
       <c r="P3" s="263">
         <f>Calculations!P3/SUM(Calculations!P$2:P$6)</f>
-        <v>0.85648003537295525</v>
+        <v>0.86192177546907589</v>
       </c>
       <c r="Q3" s="263">
         <f>Calculations!Q3/SUM(Calculations!Q$2:Q$6)</f>
-        <v>0.84846677626178246</v>
+        <v>0.85381407677707255</v>
       </c>
       <c r="R3" s="263">
         <f>Calculations!R3/SUM(Calculations!R$2:R$6)</f>
-        <v>0.84049243469864843</v>
+        <v>0.84574569089357365</v>
       </c>
       <c r="S3" s="263">
         <f>Calculations!S3/SUM(Calculations!S$2:S$6)</f>
-        <v>0.83255672785732249</v>
+        <v>0.83771633257875122</v>
       </c>
       <c r="T3" s="263">
         <f>Calculations!T3/SUM(Calculations!T$2:T$6)</f>
-        <v>0.82465937564546976</v>
+        <v>0.82972571934558526</v>
       </c>
       <c r="U3" s="263">
         <f>Calculations!U3/SUM(Calculations!U$2:U$6)</f>
-        <v>0.81680010067169639</v>
+        <v>0.82177357142673502</v>
       </c>
       <c r="V3" s="263">
         <f>Calculations!V3/SUM(Calculations!V$2:V$6)</f>
-        <v>0.80897862821307198</v>
+        <v>0.81385961174188726</v>
       </c>
       <c r="W3" s="263">
         <f>Calculations!W3/SUM(Calculations!W$2:W$6)</f>
-        <v>0.79981723129954496</v>
+        <v>0.80459756381552483</v>
       </c>
       <c r="X3" s="263">
         <f>Calculations!X3/SUM(Calculations!X$2:X$6)</f>
-        <v>0.79070684925773305</v>
+        <v>0.7953871992663466</v>
       </c>
       <c r="Y3" s="263">
         <f>Calculations!Y3/SUM(Calculations!Y$2:Y$6)</f>
-        <v>0.78164705715933036</v>
+        <v>0.78622808669848332</v>
       </c>
       <c r="Z3" s="263">
         <f>Calculations!Z3/SUM(Calculations!Z$2:Z$6)</f>
-        <v>0.77263743478221658</v>
+        <v>0.77711979950383392</v>
       </c>
       <c r="AA3" s="263">
         <f>Calculations!AA3/SUM(Calculations!AA$2:AA$6)</f>
-        <v>0.76367756654548558</v>
+        <v>0.76806191579583016</v>
       </c>
       <c r="AB3" s="263">
         <f>Calculations!AB3/SUM(Calculations!AB$2:AB$6)</f>
-        <v>0.75476704144554496</v>
+        <v>0.75905401834429576</v>
       </c>
       <c r="AC3" s="263">
         <f>Calculations!AC3/SUM(Calculations!AC$2:AC$6)</f>
-        <v>0.74590545299326994</v>
+        <v>0.75009569451138225</v>
       </c>
       <c r="AD3" s="263">
         <f>Calculations!AD3/SUM(Calculations!AD$2:AD$6)</f>
-        <v>0.73709239915218905</v>
+        <v>0.74118653618855967</v>
       </c>
       <c r="AE3" s="263">
         <f>Calculations!AE3/SUM(Calculations!AE$2:AE$6)</f>
-        <v>0.72832748227768362</v>
+        <v>0.73232613973464189</v>
       </c>
       <c r="AF3" s="263">
         <f>Calculations!AF3/SUM(Calculations!AF$2:AF$6)</f>
-        <v>0.71961030905717971</v>
+        <v>0.72351410591482535</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.35">
@@ -22247,127 +22245,127 @@
       </c>
       <c r="B6" s="263">
         <f>Calculations!B6/SUM(Calculations!B$2:B$6)</f>
-        <v>0.11414747707927995</v>
+        <v>0.107922851132606</v>
       </c>
       <c r="C6" s="263">
         <f>Calculations!C6/SUM(Calculations!C$2:C$6)</f>
-        <v>0.11319944057864668</v>
+        <v>0.10701403405461746</v>
       </c>
       <c r="D6" s="263">
         <f>Calculations!D6/SUM(Calculations!D$2:D$6)</f>
-        <v>0.11225170420120803</v>
+        <v>0.10610562335878651</v>
       </c>
       <c r="E6" s="263">
         <f>Calculations!E6/SUM(Calculations!E$2:E$6)</f>
-        <v>0.11130426780447</v>
+        <v>0.10519761877260041</v>
       </c>
       <c r="F6" s="263">
         <f>Calculations!F6/SUM(Calculations!F$2:F$6)</f>
-        <v>0.11035713124602875</v>
+        <v>0.10429002002378983</v>
       </c>
       <c r="G6" s="263">
         <f>Calculations!G6/SUM(Calculations!G$2:G$6)</f>
-        <v>0.10941029438357065</v>
+        <v>0.10338282684032898</v>
       </c>
       <c r="H6" s="263">
         <f>Calculations!H6/SUM(Calculations!H$2:H$6)</f>
-        <v>0.10846375707487201</v>
+        <v>0.10247603895043496</v>
       </c>
       <c r="I6" s="263">
         <f>Calculations!I6/SUM(Calculations!I$2:I$6)</f>
-        <v>0.10751751917779914</v>
+        <v>0.10156965608256767</v>
       </c>
       <c r="J6" s="263">
         <f>Calculations!J6/SUM(Calculations!J$2:J$6)</f>
-        <v>0.10657158055030838</v>
+        <v>0.10066367796542969</v>
       </c>
       <c r="K6" s="263">
         <f>Calculations!K6/SUM(Calculations!K$2:K$6)</f>
-        <v>0.10562594105044569</v>
+        <v>9.9758104327965599E-2</v>
       </c>
       <c r="L6" s="263">
         <f>Calculations!L6/SUM(Calculations!L$2:L$6)</f>
-        <v>0.10468060053634697</v>
+        <v>9.8852934899362171E-2</v>
       </c>
       <c r="M6" s="263">
         <f>Calculations!M6/SUM(Calculations!M$2:M$6)</f>
-        <v>0.1030124288668587</v>
+        <v>9.7274329814235685E-2</v>
       </c>
       <c r="N6" s="263">
         <f>Calculations!N6/SUM(Calculations!N$2:N$6)</f>
-        <v>0.10135243837974457</v>
+        <v>9.570345406459238E-2</v>
       </c>
       <c r="O6" s="263">
         <f>Calculations!O6/SUM(Calculations!O$2:O$6)</f>
-        <v>9.970056903799969E-2</v>
+        <v>9.4140251021267399E-2</v>
       </c>
       <c r="P6" s="263">
         <f>Calculations!P6/SUM(Calculations!P$2:P$6)</f>
-        <v>9.8056761390621888E-2</v>
+        <v>9.258466460694148E-2</v>
       </c>
       <c r="Q6" s="263">
         <f>Calculations!Q6/SUM(Calculations!Q$2:Q$6)</f>
-        <v>9.6420956565479415E-2</v>
+        <v>9.1036639289435103E-2</v>
       </c>
       <c r="R6" s="263">
         <f>Calculations!R6/SUM(Calculations!R$2:R$6)</f>
-        <v>9.4793096262282509E-2</v>
+        <v>8.9496120075100424E-2</v>
       </c>
       <c r="S6" s="263">
         <f>Calculations!S6/SUM(Calculations!S$2:S$6)</f>
-        <v>9.3173122745657061E-2</v>
+        <v>8.7963052502308819E-2</v>
       </c>
       <c r="T6" s="263">
         <f>Calculations!T6/SUM(Calculations!T$2:T$6)</f>
-        <v>9.1560978838319013E-2</v>
+        <v>8.6437382635032881E-2</v>
       </c>
       <c r="U6" s="263">
         <f>Calculations!U6/SUM(Calculations!U$2:U$6)</f>
-        <v>8.9956607914346925E-2</v>
+        <v>8.4919057056521058E-2</v>
       </c>
       <c r="V6" s="263">
         <f>Calculations!V6/SUM(Calculations!V$2:V$6)</f>
-        <v>8.8359953892552218E-2</v>
+        <v>8.3408022863063397E-2</v>
       </c>
       <c r="W6" s="263">
         <f>Calculations!W6/SUM(Calculations!W$2:W$6)</f>
-        <v>8.661381748557484E-2</v>
+        <v>8.1755667843673774E-2</v>
       </c>
       <c r="X6" s="263">
         <f>Calculations!X6/SUM(Calculations!X$2:X$6)</f>
-        <v>8.4877404369230983E-2</v>
+        <v>8.0112533170409367E-2</v>
       </c>
       <c r="Y6" s="263">
         <f>Calculations!Y6/SUM(Calculations!Y$2:Y$6)</f>
-        <v>8.3150633553384229E-2</v>
+        <v>7.8478541881983027E-2</v>
       </c>
       <c r="Z6" s="263">
         <f>Calculations!Z6/SUM(Calculations!Z$2:Z$6)</f>
-        <v>8.1433424944883967E-2</v>
+        <v>7.685361787124842E-2</v>
       </c>
       <c r="AA6" s="263">
         <f>Calculations!AA6/SUM(Calculations!AA$2:AA$6)</f>
-        <v>7.9725699335181838E-2</v>
+        <v>7.5237685873383489E-2</v>
       </c>
       <c r="AB6" s="263">
         <f>Calculations!AB6/SUM(Calculations!AB$2:AB$6)</f>
-        <v>7.8027378388152588E-2</v>
+        <v>7.3630671454269422E-2</v>
       </c>
       <c r="AC6" s="263">
         <f>Calculations!AC6/SUM(Calculations!AC$2:AC$6)</f>
-        <v>7.6338384628115763E-2</v>
+        <v>7.2032500999061513E-2</v>
       </c>
       <c r="AD6" s="263">
         <f>Calculations!AD6/SUM(Calculations!AD$2:AD$6)</f>
-        <v>7.4658641428054076E-2</v>
+        <v>7.0443101700948169E-2</v>
       </c>
       <c r="AE6" s="263">
         <f>Calculations!AE6/SUM(Calculations!AE$2:AE$6)</f>
-        <v>7.2988072998024997E-2</v>
+        <v>6.886240155009471E-2</v>
       </c>
       <c r="AF6" s="263">
         <f>Calculations!AF6/SUM(Calculations!AF$2:AF$6)</f>
-        <v>7.1326604373761454E-2</v>
+        <v>6.7290329322767836E-2</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.35">
@@ -22572,12 +22570,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22810,20 +22810,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEA4C8E-9D8C-453A-8E5F-02C5C3A31D99}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D3E8F0-5A13-4AED-8799-E0B85C663863}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -22848,12 +22849,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D3E8F0-5A13-4AED-8799-E0B85C663863}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEA4C8E-9D8C-453A-8E5F-02C5C3A31D99}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>